<commit_message>
Adding data for 2014 and fixing column sizes.
</commit_message>
<xml_diff>
--- a/Bookkeeping.xlsx
+++ b/Bookkeeping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="18735" windowHeight="8340" tabRatio="873" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="18735" windowHeight="8340" tabRatio="873"/>
   </bookViews>
   <sheets>
     <sheet name="Targets" sheetId="15" r:id="rId1"/>
@@ -356,19 +356,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="13">
-    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="#,##0.0\ \k\W&quot;h&quot;"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ \L\ "/>
-    <numFmt numFmtId="166" formatCode="#,##0.0000\ &quot;m&quot;\³"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00\ &quot;€&quot;&quot;/m²&quot;;\-#,##0.00\ &quot;€&quot;&quot;/m²&quot;"/>
-    <numFmt numFmtId="170" formatCode="#,##0.00\ &quot;€&quot;&quot;/m³&quot;;\-#,##0.00\ &quot;€&quot;&quot;/m³&quot;"/>
-    <numFmt numFmtId="171" formatCode="#,##0.00\ &quot;m&quot;\³"/>
-    <numFmt numFmtId="172" formatCode="#,##0.00\ &quot;m&quot;\²"/>
-    <numFmt numFmtId="173" formatCode="#,##0.000000\ \k\W&quot;h&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0\ \k\W&quot;h&quot;"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00\ \L\ "/>
+    <numFmt numFmtId="170" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="171" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="#,##0.00\ &quot;€&quot;&quot;/m²&quot;;\-#,##0.00\ &quot;€&quot;&quot;/m²&quot;"/>
+    <numFmt numFmtId="173" formatCode="#,##0.00\ &quot;€&quot;&quot;/m³&quot;;\-#,##0.00\ &quot;€&quot;&quot;/m³&quot;"/>
+    <numFmt numFmtId="174" formatCode="#,##0.00\ &quot;m&quot;\³"/>
+    <numFmt numFmtId="175" formatCode="#,##0.00\ &quot;m&quot;\²"/>
+    <numFmt numFmtId="176" formatCode="#,##0.000000\ \k\W&quot;h&quot;"/>
+    <numFmt numFmtId="177" formatCode="#,##0.000\ &quot;m&quot;\³"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -789,7 +789,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -799,8 +799,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -818,49 +818,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="6" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -879,7 +879,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -887,7 +887,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -897,7 +897,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -916,14 +916,14 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -949,25 +949,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
@@ -989,19 +989,19 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1010,25 +1010,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
@@ -1044,22 +1044,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1077,8 +1068,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1104,7 +1095,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1177,6 +1168,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1186,19 +1192,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1264,7 +1264,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -1388,7 +1388,7 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="5"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
@@ -1397,6 +1397,72 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>2013</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Targets!$W$16:$W$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.7619047619047624E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17523809523809525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.21333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28190476190476188</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.37333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45714285714285713</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.70095238095238099</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.78476190476190477</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.86857142857142855</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95238095238095233</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0361904761904761</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Targets!$X$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1460,45 +1526,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Targets!$W$17:$W$28</c:f>
+              <c:f>Targets!$X$17:$X$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>8.7619047619047624E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17523809523809525</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21333333333333335</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.28190476190476188</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.37333333333333335</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.45714285714285713</c:v>
+                  <c:v>0.34499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70095238095238099</c:v>
+                  <c:v>0.23499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.78476190476190477</c:v>
+                  <c:v>7.4999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.86857142857142855</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.95238095238095233</c:v>
+                  <c:v>-0.105</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0361904761904761</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1506,7 +1572,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Targets!$T$15</c:f>
@@ -1613,7 +1679,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Targets!$S$15</c:f>
@@ -1720,7 +1786,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Targets!$U$15</c:f>
@@ -1826,24 +1892,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50914432"/>
-        <c:axId val="50915968"/>
+        <c:axId val="55214848"/>
+        <c:axId val="55216384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50914432"/>
+        <c:axId val="55214848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50915968"/>
+        <c:crossAx val="55216384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50915968"/>
+        <c:axId val="55216384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1852,7 +1918,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50914432"/>
+        <c:crossAx val="55214848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1870,7 +1936,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001354" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001354" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1878,7 +1944,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -2117,24 +2183,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51739648"/>
-        <c:axId val="51745536"/>
+        <c:axId val="55126656"/>
+        <c:axId val="55173504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51739648"/>
+        <c:axId val="55126656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51745536"/>
+        <c:crossAx val="55173504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51745536"/>
+        <c:axId val="55173504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2142,7 +2208,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51739648"/>
+        <c:crossAx val="55126656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2155,7 +2221,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000777" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000777" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000788" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000788" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2684,10 +2750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W28"/>
+  <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2697,71 +2763,74 @@
     <col min="16" max="18" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
-      <c r="A1" s="150" t="s">
+    <row r="1" spans="1:24">
+      <c r="A1" s="147" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
-      <c r="G1" s="150"/>
-      <c r="H1" s="150"/>
-      <c r="I1" s="150"/>
-      <c r="J1" s="150"/>
-      <c r="K1" s="150"/>
-      <c r="L1" s="150"/>
-      <c r="M1" s="150"/>
-      <c r="N1" s="150"/>
-    </row>
-    <row r="9" spans="1:23">
-      <c r="P9" s="149"/>
-      <c r="Q9" s="149"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="J1" s="147"/>
+      <c r="K1" s="147"/>
+      <c r="L1" s="147"/>
+      <c r="M1" s="147"/>
+      <c r="N1" s="147"/>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="P9" s="146"/>
+      <c r="Q9" s="146"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:23">
-      <c r="P10" s="149"/>
-      <c r="Q10" s="149"/>
+    <row r="10" spans="1:24">
+      <c r="P10" s="146"/>
+      <c r="Q10" s="146"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:23">
-      <c r="P11" s="149"/>
-      <c r="Q11" s="149"/>
+    <row r="11" spans="1:24">
+      <c r="P11" s="146"/>
+      <c r="Q11" s="146"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:23">
-      <c r="P12" s="149"/>
-      <c r="Q12" s="149"/>
+    <row r="12" spans="1:24">
+      <c r="P12" s="146"/>
+      <c r="Q12" s="146"/>
       <c r="R12" s="49"/>
     </row>
-    <row r="15" spans="1:23">
-      <c r="P15" s="141" t="s">
+    <row r="15" spans="1:24">
+      <c r="P15" s="138" t="s">
         <v>90</v>
       </c>
-      <c r="Q15" s="141" t="s">
+      <c r="Q15" s="138" t="s">
         <v>91</v>
       </c>
-      <c r="R15" s="141" t="s">
+      <c r="R15" s="138" t="s">
         <v>92</v>
       </c>
-      <c r="S15" s="141" t="s">
+      <c r="S15" s="138" t="s">
         <v>90</v>
       </c>
-      <c r="T15" s="141" t="s">
+      <c r="T15" s="138" t="s">
         <v>91</v>
       </c>
-      <c r="U15" s="141" t="s">
+      <c r="U15" s="138" t="s">
         <v>92</v>
       </c>
-      <c r="V15" s="141">
+      <c r="V15" s="138">
         <v>2012</v>
       </c>
       <c r="W15">
         <v>2013</v>
       </c>
-    </row>
-    <row r="16" spans="1:23">
+      <c r="X15">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="P16" s="3">
         <v>0</v>
       </c>
@@ -2787,9 +2856,12 @@
       <c r="W16" s="117">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="15:23">
-      <c r="O17" s="140" t="s">
+      <c r="X16" s="117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="15:24">
+      <c r="O17" s="137" t="s">
         <v>49</v>
       </c>
       <c r="P17" s="3">
@@ -2821,9 +2893,12 @@
       <c r="W17" s="117">
         <v>8.7619047619047624E-2</v>
       </c>
-    </row>
-    <row r="18" spans="15:23">
-      <c r="O18" s="140" t="s">
+      <c r="X17" s="117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="15:24">
+      <c r="O18" s="137" t="s">
         <v>50</v>
       </c>
       <c r="P18" s="3">
@@ -2856,9 +2931,12 @@
       <c r="W18" s="117">
         <v>0.17523809523809525</v>
       </c>
-    </row>
-    <row r="19" spans="15:23">
-      <c r="O19" s="140" t="s">
+      <c r="X18" s="117">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19" spans="15:24">
+      <c r="O19" s="137" t="s">
         <v>51</v>
       </c>
       <c r="P19" s="3">
@@ -2891,9 +2969,12 @@
       <c r="W19" s="117">
         <v>0.21333333333333335</v>
       </c>
-    </row>
-    <row r="20" spans="15:23">
-      <c r="O20" s="140" t="s">
+      <c r="X19" s="117">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="15:24">
+      <c r="O20" s="137" t="s">
         <v>52</v>
       </c>
       <c r="P20" s="3">
@@ -2926,9 +3007,12 @@
       <c r="W20" s="117">
         <v>0.28190476190476188</v>
       </c>
-    </row>
-    <row r="21" spans="15:23">
-      <c r="O21" s="140" t="s">
+      <c r="X20" s="117">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="21" spans="15:24">
+      <c r="O21" s="137" t="s">
         <v>53</v>
       </c>
       <c r="P21" s="3">
@@ -2961,9 +3045,12 @@
       <c r="W21" s="117">
         <v>0.37333333333333335</v>
       </c>
-    </row>
-    <row r="22" spans="15:23">
-      <c r="O22" s="140" t="s">
+      <c r="X21" s="117">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="22" spans="15:24">
+      <c r="O22" s="137" t="s">
         <v>54</v>
       </c>
       <c r="P22" s="3">
@@ -2996,9 +3083,12 @@
       <c r="W22" s="117">
         <v>0.45714285714285713</v>
       </c>
-    </row>
-    <row r="23" spans="15:23">
-      <c r="O23" s="140" t="s">
+      <c r="X22" s="117">
+        <v>0.34499999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="15:24">
+      <c r="O23" s="137" t="s">
         <v>55</v>
       </c>
       <c r="P23" s="3">
@@ -3031,9 +3121,12 @@
       <c r="W23" s="117">
         <v>0.70095238095238099</v>
       </c>
-    </row>
-    <row r="24" spans="15:23">
-      <c r="O24" s="140" t="s">
+      <c r="X23" s="117">
+        <v>0.23499999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="15:24">
+      <c r="O24" s="137" t="s">
         <v>56</v>
       </c>
       <c r="P24" s="3">
@@ -3066,9 +3159,12 @@
       <c r="W24" s="117">
         <v>0.78476190476190477</v>
       </c>
-    </row>
-    <row r="25" spans="15:23">
-      <c r="O25" s="140" t="s">
+      <c r="X24" s="117">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="15:24">
+      <c r="O25" s="137" t="s">
         <v>57</v>
       </c>
       <c r="P25" s="3">
@@ -3101,9 +3197,12 @@
       <c r="W25" s="117">
         <v>0.86857142857142855</v>
       </c>
-    </row>
-    <row r="26" spans="15:23">
-      <c r="O26" s="140" t="s">
+      <c r="X25" s="117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="15:24">
+      <c r="O26" s="137" t="s">
         <v>58</v>
       </c>
       <c r="P26" s="3">
@@ -3136,9 +3235,12 @@
       <c r="W26" s="117">
         <v>0.95238095238095233</v>
       </c>
-    </row>
-    <row r="27" spans="15:23">
-      <c r="O27" s="140" t="s">
+      <c r="X26" s="117">
+        <v>-0.105</v>
+      </c>
+    </row>
+    <row r="27" spans="15:24">
+      <c r="O27" s="137" t="s">
         <v>59</v>
       </c>
       <c r="P27" s="3">
@@ -3171,9 +3273,12 @@
       <c r="W27" s="117">
         <v>1.0361904761904761</v>
       </c>
-    </row>
-    <row r="28" spans="15:23">
-      <c r="O28" s="140" t="s">
+      <c r="X27" s="117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="15:24">
+      <c r="O28" s="137" t="s">
         <v>60</v>
       </c>
       <c r="P28" s="3">
@@ -3204,6 +3309,9 @@
       </c>
       <c r="W28" s="117">
         <v>1.1200000000000001</v>
+      </c>
+      <c r="X28" s="117">
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3226,7 +3334,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="132" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="129" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
@@ -3254,14 +3362,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="172"/>
+      <c r="M2" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="172"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3292,12 +3400,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="170"/>
+      <c r="B4" s="171"/>
+      <c r="C4" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="174"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3324,8 +3432,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="170"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3341,10 +3449,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="170" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3357,10 +3465,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3370,10 +3478,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="170" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3383,10 +3491,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3396,8 +3504,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="170"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3408,8 +3516,8 @@
       <c r="F10" s="49"/>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="170"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3420,8 +3528,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -3435,13 +3543,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -3483,12 +3591,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -3496,6 +3598,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3515,7 +3623,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="132" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="129" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
@@ -3543,14 +3651,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="172"/>
+      <c r="M2" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="172"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3581,12 +3689,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="170"/>
+      <c r="B4" s="171"/>
+      <c r="C4" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="174"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3613,8 +3721,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="170"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3630,8 +3738,8 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176"/>
-      <c r="B6" s="177"/>
+      <c r="A6" s="170"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3644,10 +3752,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3658,10 +3766,10 @@
       <c r="E7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="170" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3671,10 +3779,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="170" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3684,8 +3792,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="170"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3695,8 +3803,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="170"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3708,8 +3816,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -3722,13 +3830,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -3770,12 +3878,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -3783,6 +3885,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3802,7 +3910,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="132" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="129" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
@@ -3831,14 +3939,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="172"/>
+      <c r="M2" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="172"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3869,12 +3977,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="170"/>
+      <c r="B4" s="171"/>
+      <c r="C4" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="174"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3901,8 +4009,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="170"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3918,10 +4026,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="170" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3934,10 +4042,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="170" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3947,10 +4055,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3960,10 +4068,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3973,10 +4081,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="170" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3986,8 +4094,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="170"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3998,8 +4106,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4015,13 +4123,13 @@
       <c r="O13" s="49"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -4063,12 +4171,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4076,6 +4178,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4095,7 +4203,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="131" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="128" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
@@ -4122,14 +4230,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="172"/>
+      <c r="M2" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="172"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4160,12 +4268,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="170"/>
+      <c r="B4" s="171"/>
+      <c r="C4" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="174"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4192,8 +4300,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="170"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4209,10 +4317,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4225,10 +4333,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="170" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4238,10 +4346,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4251,10 +4359,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="170" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4264,10 +4372,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="170" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4277,8 +4385,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="170"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4290,8 +4398,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4306,13 +4414,13 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="121" t="s">
@@ -4354,12 +4462,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4367,6 +4469,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4414,14 +4522,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="172"/>
+      <c r="M2" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="172"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4452,14 +4560,14 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="170" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="171"/>
+      <c r="C4" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="174"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4486,10 +4594,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4505,10 +4613,10 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="170" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4521,10 +4629,10 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4534,10 +4642,10 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4547,10 +4655,10 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="170" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4560,10 +4668,10 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4573,10 +4681,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="170" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4588,8 +4696,8 @@
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4603,13 +4711,13 @@
     </row>
     <row r="13" spans="1:16" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="121" t="s">
@@ -4651,12 +4759,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4664,6 +4766,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4710,14 +4818,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="172"/>
+      <c r="M2" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="172"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4748,12 +4856,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="170"/>
+      <c r="B4" s="171"/>
+      <c r="C4" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="174"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4780,10 +4888,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="170" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4798,10 +4906,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="170" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4813,10 +4921,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="170" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4826,10 +4934,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4839,10 +4947,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="170" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4852,10 +4960,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4865,10 +4973,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="170" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4879,8 +4987,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4894,13 +5002,13 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="121" t="s">
@@ -4968,9 +5076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4988,16 +5094,16 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:13">
-      <c r="A2" s="154">
+      <c r="A2" s="151">
         <v>2012</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="156"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="H2" s="153"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1">
       <c r="A3" s="19"/>
@@ -5020,18 +5126,18 @@
       <c r="H3" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="151" t="s">
+      <c r="J3" s="148" t="s">
         <v>103</v>
       </c>
-      <c r="K3" s="151"/>
-      <c r="L3" s="151"/>
-      <c r="M3" s="151"/>
+      <c r="K3" s="148"/>
+      <c r="L3" s="148"/>
+      <c r="M3" s="148"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="161" t="s">
+      <c r="A4" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="162"/>
+      <c r="B4" s="159"/>
       <c r="C4" s="21">
         <f>January!$D7</f>
         <v>0</v>
@@ -5056,22 +5162,22 @@
         <f>June!$D7</f>
         <v>0</v>
       </c>
-      <c r="J4" s="142"/>
-      <c r="K4" s="143" t="s">
+      <c r="J4" s="139"/>
+      <c r="K4" s="140" t="s">
         <v>97</v>
       </c>
-      <c r="L4" s="143" t="s">
+      <c r="L4" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="M4" s="144" t="s">
+      <c r="M4" s="141" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="161" t="s">
+      <c r="A5" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="162"/>
+      <c r="B5" s="159"/>
       <c r="C5" s="28">
         <f>January!$D8</f>
         <v>0</v>
@@ -5096,14 +5202,14 @@
         <f>June!$D8</f>
         <v>0</v>
       </c>
-      <c r="J5" s="145" t="s">
+      <c r="J5" s="142" t="s">
         <v>49</v>
       </c>
-      <c r="K5" s="146">
+      <c r="K5" s="143">
         <f>C$4+C$5</f>
         <v>0</v>
       </c>
-      <c r="L5" s="146">
+      <c r="L5" s="143">
         <f>C$6+C$7</f>
         <v>0</v>
       </c>
@@ -5113,10 +5219,10 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="161" t="s">
+      <c r="A6" s="158" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="162"/>
+      <c r="B6" s="159"/>
       <c r="C6" s="24">
         <f>January!$D9</f>
         <v>0</v>
@@ -5141,14 +5247,14 @@
         <f>June!$D9</f>
         <v>0</v>
       </c>
-      <c r="J6" s="145" t="s">
+      <c r="J6" s="142" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="146">
+      <c r="K6" s="143">
         <f>D$4+D$5</f>
         <v>0</v>
       </c>
-      <c r="L6" s="146">
+      <c r="L6" s="143">
         <f>D$6+D$7</f>
         <v>0</v>
       </c>
@@ -5158,10 +5264,10 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="161" t="s">
+      <c r="A7" s="158" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="162"/>
+      <c r="B7" s="159"/>
       <c r="C7" s="28">
         <f>January!$D10</f>
         <v>0</v>
@@ -5186,14 +5292,14 @@
         <f>June!$D10</f>
         <v>0</v>
       </c>
-      <c r="J7" s="145" t="s">
+      <c r="J7" s="142" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="146">
+      <c r="K7" s="143">
         <f>E$4+E$5</f>
         <v>0</v>
       </c>
-      <c r="L7" s="146">
+      <c r="L7" s="143">
         <f>E$6+E$7</f>
         <v>0</v>
       </c>
@@ -5203,10 +5309,10 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="161" t="s">
+      <c r="A8" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="162"/>
+      <c r="B8" s="159"/>
       <c r="C8" s="24">
         <f>January!$D11</f>
         <v>0</v>
@@ -5231,14 +5337,14 @@
         <f>June!$D11</f>
         <v>0</v>
       </c>
-      <c r="J8" s="145" t="s">
+      <c r="J8" s="142" t="s">
         <v>52</v>
       </c>
-      <c r="K8" s="146">
+      <c r="K8" s="143">
         <f>F$4+F$5</f>
         <v>0</v>
       </c>
-      <c r="L8" s="146">
+      <c r="L8" s="143">
         <f>F$6+F$7</f>
         <v>0</v>
       </c>
@@ -5248,10 +5354,10 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A9" s="161" t="s">
+      <c r="A9" s="158" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="162"/>
+      <c r="B9" s="159"/>
       <c r="C9" s="27">
         <f>January!$D12</f>
         <v>0</v>
@@ -5276,14 +5382,14 @@
         <f>June!$D12</f>
         <v>0</v>
       </c>
-      <c r="J9" s="145" t="s">
+      <c r="J9" s="142" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="146">
+      <c r="K9" s="143">
         <f>G$4+G$5</f>
         <v>0</v>
       </c>
-      <c r="L9" s="146">
+      <c r="L9" s="143">
         <f>G$6+G$7</f>
         <v>0</v>
       </c>
@@ -5313,14 +5419,14 @@
       <c r="H10" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="145" t="s">
+      <c r="J10" s="142" t="s">
         <v>54</v>
       </c>
-      <c r="K10" s="146">
+      <c r="K10" s="143">
         <f>H$4+H$5</f>
         <v>0</v>
       </c>
-      <c r="L10" s="146">
+      <c r="L10" s="143">
         <f>H$6+H$7</f>
         <v>0</v>
       </c>
@@ -5330,10 +5436,10 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="161" t="s">
+      <c r="A11" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="162"/>
+      <c r="B11" s="159"/>
       <c r="C11" s="22">
         <f>July!$D7</f>
         <v>0</v>
@@ -5358,14 +5464,14 @@
         <f>December!$D7</f>
         <v>0</v>
       </c>
-      <c r="J11" s="145" t="s">
+      <c r="J11" s="142" t="s">
         <v>55</v>
       </c>
-      <c r="K11" s="146">
+      <c r="K11" s="143">
         <f>C$11+C$12</f>
         <v>0</v>
       </c>
-      <c r="L11" s="146">
+      <c r="L11" s="143">
         <f>C$13+C$14</f>
         <v>0</v>
       </c>
@@ -5375,10 +5481,10 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="161" t="s">
+      <c r="A12" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="162"/>
+      <c r="B12" s="159"/>
       <c r="C12" s="29">
         <f>July!$D8</f>
         <v>0</v>
@@ -5403,14 +5509,14 @@
         <f>December!$D8</f>
         <v>0</v>
       </c>
-      <c r="J12" s="145" t="s">
+      <c r="J12" s="142" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="146">
+      <c r="K12" s="143">
         <f>D$11+D$12</f>
         <v>0</v>
       </c>
-      <c r="L12" s="146">
+      <c r="L12" s="143">
         <f>D$13+D$14</f>
         <v>0</v>
       </c>
@@ -5420,10 +5526,10 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="161" t="s">
+      <c r="A13" s="158" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="162"/>
+      <c r="B13" s="159"/>
       <c r="C13" s="25">
         <f>July!$D9</f>
         <v>0</v>
@@ -5448,14 +5554,14 @@
         <f>December!$D9</f>
         <v>0</v>
       </c>
-      <c r="J13" s="145" t="s">
+      <c r="J13" s="142" t="s">
         <v>57</v>
       </c>
-      <c r="K13" s="146">
+      <c r="K13" s="143">
         <f>E$11+E$12</f>
         <v>0</v>
       </c>
-      <c r="L13" s="146">
+      <c r="L13" s="143">
         <f>E$13+E$14</f>
         <v>0</v>
       </c>
@@ -5465,10 +5571,10 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="161" t="s">
+      <c r="A14" s="158" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="162"/>
+      <c r="B14" s="159"/>
       <c r="C14" s="29">
         <f>July!$D10</f>
         <v>0</v>
@@ -5493,14 +5599,14 @@
         <f>December!$D10</f>
         <v>0</v>
       </c>
-      <c r="J14" s="145" t="s">
+      <c r="J14" s="142" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="146">
+      <c r="K14" s="143">
         <f>F$11+F$12</f>
         <v>0</v>
       </c>
-      <c r="L14" s="146">
+      <c r="L14" s="143">
         <f>F$13+F$14</f>
         <v>0</v>
       </c>
@@ -5510,10 +5616,10 @@
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="161" t="s">
+      <c r="A15" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="162"/>
+      <c r="B15" s="159"/>
       <c r="C15" s="25">
         <f>July!$D11</f>
         <v>0</v>
@@ -5538,14 +5644,14 @@
         <f>December!$D11</f>
         <v>0</v>
       </c>
-      <c r="J15" s="145" t="s">
+      <c r="J15" s="142" t="s">
         <v>59</v>
       </c>
-      <c r="K15" s="146">
+      <c r="K15" s="143">
         <f>G$11+G$12</f>
         <v>0</v>
       </c>
-      <c r="L15" s="146">
+      <c r="L15" s="143">
         <f>G$13+G$14</f>
         <v>0</v>
       </c>
@@ -5555,10 +5661,10 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A16" s="152" t="s">
+      <c r="A16" s="149" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="153"/>
+      <c r="B16" s="150"/>
       <c r="C16" s="31">
         <f>July!$D12</f>
         <v>0</v>
@@ -5583,14 +5689,14 @@
         <f>December!$D12</f>
         <v>0</v>
       </c>
-      <c r="J16" s="145" t="s">
+      <c r="J16" s="142" t="s">
         <v>60</v>
       </c>
-      <c r="K16" s="146">
+      <c r="K16" s="143">
         <f>H$11+H$12</f>
         <v>0</v>
       </c>
-      <c r="L16" s="146">
+      <c r="L16" s="143">
         <f>H$13+H$14</f>
         <v>0</v>
       </c>
@@ -5600,9 +5706,9 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1">
-      <c r="J17" s="147"/>
-      <c r="K17" s="148"/>
-      <c r="L17" s="148" t="s">
+      <c r="J17" s="144"/>
+      <c r="K17" s="145"/>
+      <c r="L17" s="145" t="s">
         <v>93</v>
       </c>
       <c r="M17" s="18">
@@ -5611,23 +5717,23 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="157" t="s">
+      <c r="A18" s="154" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="158"/>
-      <c r="C18" s="159"/>
-      <c r="D18" s="133" t="e">
+      <c r="B18" s="155"/>
+      <c r="C18" s="156"/>
+      <c r="D18" s="130" t="e">
         <f>AVERAGEIF(K5:K16,"&gt;0")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A19" s="152" t="s">
+      <c r="A19" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="160"/>
-      <c r="C19" s="153"/>
-      <c r="D19" s="134" t="e">
+      <c r="B19" s="157"/>
+      <c r="C19" s="150"/>
+      <c r="D19" s="131" t="e">
         <f>AVERAGEIF(L5:L16,"&gt;0")</f>
         <v>#DIV/0!</v>
       </c>
@@ -5663,50 +5769,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:T32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" customWidth="1"/>
     <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.140625" customWidth="1"/>
-    <col min="17" max="19" width="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1">
       <c r="H1" s="49"/>
     </row>
     <row r="2" spans="2:19" ht="15.75" thickBot="1">
-      <c r="D2" s="157" t="s">
+      <c r="D2" s="154" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="159"/>
+      <c r="E2" s="156"/>
       <c r="F2" s="64">
         <v>0</v>
       </c>
-      <c r="J2" s="167" t="s">
+      <c r="J2" s="164" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="168"/>
-      <c r="L2" s="171">
+      <c r="K2" s="165"/>
+      <c r="L2" s="168">
         <v>1000</v>
       </c>
-      <c r="M2" s="172"/>
+      <c r="M2" s="169"/>
       <c r="N2" s="107"/>
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1">
@@ -5728,18 +5832,18 @@
       </c>
     </row>
     <row r="4" spans="2:19">
-      <c r="D4" s="161" t="s">
+      <c r="D4" s="158" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="162"/>
+      <c r="E4" s="159"/>
       <c r="F4" s="66">
         <v>1</v>
       </c>
       <c r="I4" s="49"/>
-      <c r="J4" s="169" t="s">
+      <c r="J4" s="166" t="s">
         <v>80</v>
       </c>
-      <c r="K4" s="166"/>
+      <c r="K4" s="163"/>
       <c r="L4" s="101">
         <v>1</v>
       </c>
@@ -5749,19 +5853,19 @@
       <c r="N4" s="108"/>
     </row>
     <row r="5" spans="2:19">
-      <c r="D5" s="161" t="s">
+      <c r="D5" s="158" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="162"/>
+      <c r="E5" s="159"/>
       <c r="F5" s="66">
         <v>0.1</v>
       </c>
       <c r="H5" s="114"/>
       <c r="I5" s="49"/>
-      <c r="J5" s="169" t="s">
+      <c r="J5" s="166" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="166"/>
+      <c r="K5" s="163"/>
       <c r="L5" s="105" t="s">
         <v>5</v>
       </c>
@@ -5780,10 +5884,10 @@
         <v>0</v>
       </c>
       <c r="H6" s="49"/>
-      <c r="J6" s="170" t="s">
+      <c r="J6" s="167" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="163"/>
+      <c r="K6" s="160"/>
       <c r="L6" s="103">
         <v>1</v>
       </c>
@@ -5836,22 +5940,22 @@
     </row>
     <row r="9" spans="2:19" ht="15.75" thickBot="1">
       <c r="B9" s="33"/>
-      <c r="C9" s="136" t="s">
+      <c r="C9" s="133" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="136" t="s">
+      <c r="D9" s="133" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="136" t="s">
+      <c r="E9" s="133" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="136" t="s">
+      <c r="F9" s="133" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="136" t="s">
+      <c r="G9" s="133" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="137" t="s">
+      <c r="H9" s="134" t="s">
         <v>64</v>
       </c>
       <c r="J9" s="33"/>
@@ -5865,10 +5969,10 @@
       <c r="N9" s="119" t="s">
         <v>85</v>
       </c>
-      <c r="O9" s="139" t="s">
+      <c r="O9" s="136" t="s">
         <v>101</v>
       </c>
-      <c r="P9" s="139" t="s">
+      <c r="P9" s="136" t="s">
         <v>102</v>
       </c>
       <c r="Q9" s="62">
@@ -5912,13 +6016,13 @@
       <c r="K10" s="34">
         <v>0</v>
       </c>
-      <c r="L10" s="128">
+      <c r="L10" s="125">
         <v>41640</v>
       </c>
-      <c r="M10" s="122">
-        <v>0</v>
-      </c>
-      <c r="N10" s="122">
+      <c r="M10" s="178">
+        <v>0</v>
+      </c>
+      <c r="N10" s="178">
         <v>0</v>
       </c>
       <c r="O10" s="53" t="s">
@@ -5938,7 +6042,7 @@
       </c>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="138" t="s">
+      <c r="B11" s="135" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="112">
@@ -5970,23 +6074,23 @@
       <c r="K11" s="37">
         <v>0</v>
       </c>
-      <c r="L11" s="129">
+      <c r="L11" s="126">
         <f t="shared" ref="L11:L14" si="5">L10+1</f>
         <v>41641</v>
       </c>
-      <c r="M11" s="123">
+      <c r="M11" s="179">
         <f t="shared" ref="M11:N22" si="6">M10</f>
         <v>0</v>
       </c>
-      <c r="N11" s="123">
+      <c r="N11" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O11" s="124">
+      <c r="O11" s="122">
         <f t="shared" ref="O11:O15" si="7">((M11-M10)/(L11-L10))*1000</f>
         <v>0</v>
       </c>
-      <c r="P11" s="124">
+      <c r="P11" s="122">
         <f t="shared" ref="P11:P12" si="8">((N11-N10)/(L11-L10))*1000</f>
         <v>0</v>
       </c>
@@ -5995,7 +6099,7 @@
       <c r="S11" s="70"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="138" t="s">
+      <c r="B12" s="135" t="s">
         <v>50</v>
       </c>
       <c r="C12" s="112">
@@ -6027,23 +6131,23 @@
       <c r="K12" s="37">
         <v>0</v>
       </c>
-      <c r="L12" s="129">
+      <c r="L12" s="126">
         <f t="shared" si="5"/>
         <v>41642</v>
       </c>
-      <c r="M12" s="123">
+      <c r="M12" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N12" s="123">
+      <c r="N12" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O12" s="124">
+      <c r="O12" s="122">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P12" s="124">
+      <c r="P12" s="122">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -6052,7 +6156,7 @@
       <c r="S12" s="70"/>
     </row>
     <row r="13" spans="2:19">
-      <c r="B13" s="138" t="s">
+      <c r="B13" s="135" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="112">
@@ -6084,23 +6188,23 @@
       <c r="K13" s="37">
         <v>0</v>
       </c>
-      <c r="L13" s="129">
+      <c r="L13" s="126">
         <f t="shared" si="5"/>
         <v>41643</v>
       </c>
-      <c r="M13" s="123">
+      <c r="M13" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N13" s="123">
+      <c r="N13" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O13" s="124">
+      <c r="O13" s="122">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P13" s="124">
+      <c r="P13" s="122">
         <f t="shared" ref="P13:P21" si="9">((N13-N12)/(L13-L12))*1000</f>
         <v>0</v>
       </c>
@@ -6109,7 +6213,7 @@
       <c r="S13" s="70"/>
     </row>
     <row r="14" spans="2:19">
-      <c r="B14" s="138" t="s">
+      <c r="B14" s="135" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="37">
@@ -6141,23 +6245,23 @@
       <c r="K14" s="37">
         <v>0</v>
       </c>
-      <c r="L14" s="129">
+      <c r="L14" s="126">
         <f t="shared" si="5"/>
         <v>41644</v>
       </c>
-      <c r="M14" s="123">
+      <c r="M14" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N14" s="123">
+      <c r="N14" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O14" s="124">
+      <c r="O14" s="122">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P14" s="124">
+      <c r="P14" s="122">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6166,7 +6270,7 @@
       <c r="S14" s="70"/>
     </row>
     <row r="15" spans="2:19">
-      <c r="B15" s="138" t="s">
+      <c r="B15" s="135" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="37">
@@ -6198,23 +6302,23 @@
       <c r="K15" s="37">
         <v>0</v>
       </c>
-      <c r="L15" s="129">
+      <c r="L15" s="126">
         <f t="shared" ref="L15:L22" si="10">L14+1</f>
         <v>41645</v>
       </c>
-      <c r="M15" s="123">
+      <c r="M15" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N15" s="123">
+      <c r="N15" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O15" s="124">
+      <c r="O15" s="122">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P15" s="124">
+      <c r="P15" s="122">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6223,7 +6327,7 @@
       <c r="S15" s="70"/>
     </row>
     <row r="16" spans="2:19">
-      <c r="B16" s="138" t="s">
+      <c r="B16" s="135" t="s">
         <v>54</v>
       </c>
       <c r="C16" s="37">
@@ -6255,23 +6359,23 @@
       <c r="K16" s="37">
         <v>0</v>
       </c>
-      <c r="L16" s="129">
+      <c r="L16" s="126">
         <f t="shared" si="10"/>
         <v>41646</v>
       </c>
-      <c r="M16" s="123">
+      <c r="M16" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N16" s="123">
+      <c r="N16" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O16" s="124">
+      <c r="O16" s="122">
         <f t="shared" ref="O16:O22" si="11">((M16-M15)/(L16-L15))*1000</f>
         <v>0</v>
       </c>
-      <c r="P16" s="124">
+      <c r="P16" s="122">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6280,7 +6384,7 @@
       <c r="S16" s="70"/>
     </row>
     <row r="17" spans="2:20">
-      <c r="B17" s="138" t="s">
+      <c r="B17" s="135" t="s">
         <v>55</v>
       </c>
       <c r="C17" s="37">
@@ -6312,23 +6416,23 @@
       <c r="K17" s="37">
         <v>0</v>
       </c>
-      <c r="L17" s="129">
+      <c r="L17" s="126">
         <f t="shared" si="10"/>
         <v>41647</v>
       </c>
-      <c r="M17" s="123">
+      <c r="M17" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N17" s="123">
+      <c r="N17" s="179">
         <f t="shared" ref="N17:N22" si="12">N16</f>
         <v>0</v>
       </c>
-      <c r="O17" s="124">
+      <c r="O17" s="122">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P17" s="124">
+      <c r="P17" s="122">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6337,7 +6441,7 @@
       <c r="S17" s="70"/>
     </row>
     <row r="18" spans="2:20">
-      <c r="B18" s="138" t="s">
+      <c r="B18" s="135" t="s">
         <v>56</v>
       </c>
       <c r="C18" s="37">
@@ -6369,23 +6473,23 @@
       <c r="K18" s="37">
         <v>0</v>
       </c>
-      <c r="L18" s="129">
+      <c r="L18" s="126">
         <f t="shared" si="10"/>
         <v>41648</v>
       </c>
-      <c r="M18" s="123">
+      <c r="M18" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N18" s="123">
+      <c r="N18" s="179">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="O18" s="124">
+      <c r="O18" s="122">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P18" s="124">
+      <c r="P18" s="122">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6394,7 +6498,7 @@
       <c r="S18" s="70"/>
     </row>
     <row r="19" spans="2:20">
-      <c r="B19" s="138" t="s">
+      <c r="B19" s="135" t="s">
         <v>57</v>
       </c>
       <c r="C19" s="37">
@@ -6426,23 +6530,23 @@
       <c r="K19" s="37">
         <v>0</v>
       </c>
-      <c r="L19" s="129">
+      <c r="L19" s="126">
         <f t="shared" si="10"/>
         <v>41649</v>
       </c>
-      <c r="M19" s="123">
+      <c r="M19" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N19" s="123">
+      <c r="N19" s="179">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="O19" s="124">
+      <c r="O19" s="122">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P19" s="124">
+      <c r="P19" s="122">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6451,7 +6555,7 @@
       <c r="S19" s="70"/>
     </row>
     <row r="20" spans="2:20">
-      <c r="B20" s="138" t="s">
+      <c r="B20" s="135" t="s">
         <v>58</v>
       </c>
       <c r="C20" s="37">
@@ -6483,23 +6587,23 @@
       <c r="K20" s="37">
         <v>0</v>
       </c>
-      <c r="L20" s="129">
+      <c r="L20" s="126">
         <f t="shared" si="10"/>
         <v>41650</v>
       </c>
-      <c r="M20" s="123">
+      <c r="M20" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N20" s="123">
+      <c r="N20" s="179">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="O20" s="124">
+      <c r="O20" s="122">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P20" s="124">
+      <c r="P20" s="122">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6509,7 +6613,7 @@
       <c r="T20" s="58"/>
     </row>
     <row r="21" spans="2:20">
-      <c r="B21" s="138" t="s">
+      <c r="B21" s="135" t="s">
         <v>59</v>
       </c>
       <c r="C21" s="37">
@@ -6541,23 +6645,23 @@
       <c r="K21" s="37">
         <v>0</v>
       </c>
-      <c r="L21" s="129">
+      <c r="L21" s="126">
         <f t="shared" si="10"/>
         <v>41651</v>
       </c>
-      <c r="M21" s="123">
+      <c r="M21" s="179">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N21" s="123">
+      <c r="N21" s="179">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="O21" s="124">
+      <c r="O21" s="122">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P21" s="124">
+      <c r="P21" s="122">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -6566,7 +6670,7 @@
       <c r="S21" s="70"/>
     </row>
     <row r="22" spans="2:20" ht="15.75" thickBot="1">
-      <c r="B22" s="135" t="s">
+      <c r="B22" s="132" t="s">
         <v>60</v>
       </c>
       <c r="C22" s="40">
@@ -6598,23 +6702,23 @@
       <c r="K22" s="40">
         <v>0</v>
       </c>
-      <c r="L22" s="130">
+      <c r="L22" s="127">
         <f t="shared" si="10"/>
         <v>41652</v>
       </c>
-      <c r="M22" s="125">
+      <c r="M22" s="180">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N22" s="125">
+      <c r="N22" s="180">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="O22" s="126">
+      <c r="O22" s="123">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="P22" s="127">
+      <c r="P22" s="124">
         <f>((N22-N21)/(L22-L21))*1000</f>
         <v>0</v>
       </c>
@@ -6648,10 +6752,10 @@
     </row>
     <row r="25" spans="2:20">
       <c r="H25" s="57"/>
-      <c r="J25" s="164" t="s">
+      <c r="J25" s="161" t="s">
         <v>70</v>
       </c>
-      <c r="K25" s="165"/>
+      <c r="K25" s="162"/>
       <c r="L25" s="85" t="s">
         <v>88</v>
       </c>
@@ -6666,8 +6770,8 @@
     </row>
     <row r="26" spans="2:20">
       <c r="I26" s="52"/>
-      <c r="J26" s="164"/>
-      <c r="K26" s="165"/>
+      <c r="J26" s="161"/>
+      <c r="K26" s="162"/>
       <c r="L26" s="88" t="s">
         <v>89</v>
       </c>
@@ -6680,10 +6784,10 @@
       </c>
     </row>
     <row r="27" spans="2:20">
-      <c r="J27" s="164" t="s">
+      <c r="J27" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="K27" s="165"/>
+      <c r="K27" s="162"/>
       <c r="L27" s="88" t="s">
         <v>88</v>
       </c>
@@ -6697,8 +6801,8 @@
       </c>
     </row>
     <row r="28" spans="2:20">
-      <c r="J28" s="164"/>
-      <c r="K28" s="165"/>
+      <c r="J28" s="161"/>
+      <c r="K28" s="162"/>
       <c r="L28" s="88" t="s">
         <v>89</v>
       </c>
@@ -6711,10 +6815,10 @@
       </c>
     </row>
     <row r="29" spans="2:20" ht="15.75" thickBot="1">
-      <c r="J29" s="164" t="s">
+      <c r="J29" s="161" t="s">
         <v>85</v>
       </c>
-      <c r="K29" s="165"/>
+      <c r="K29" s="162"/>
       <c r="L29" s="90" t="s">
         <v>88</v>
       </c>
@@ -6730,10 +6834,10 @@
     <row r="30" spans="2:20">
       <c r="J30" s="94"/>
       <c r="K30" s="95"/>
-      <c r="L30" s="166" t="s">
+      <c r="L30" s="163" t="s">
         <v>66</v>
       </c>
-      <c r="M30" s="166"/>
+      <c r="M30" s="163"/>
       <c r="N30" s="82">
         <f>SUM(N25:N29)</f>
         <v>90.3</v>
@@ -6742,10 +6846,10 @@
     <row r="31" spans="2:20" ht="15.75" thickBot="1">
       <c r="J31" s="94"/>
       <c r="K31" s="95"/>
-      <c r="L31" s="166" t="s">
+      <c r="L31" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="M31" s="166"/>
+      <c r="M31" s="163"/>
       <c r="N31" s="18">
         <f>SUM(K10:K22)</f>
         <v>0</v>
@@ -6754,10 +6858,10 @@
     <row r="32" spans="2:20" ht="15.75" thickBot="1">
       <c r="J32" s="81"/>
       <c r="K32" s="96"/>
-      <c r="L32" s="163" t="s">
+      <c r="L32" s="160" t="s">
         <v>75</v>
       </c>
-      <c r="M32" s="163"/>
+      <c r="M32" s="160"/>
       <c r="N32" s="79">
         <f>N31-N30</f>
         <v>-90.3</v>
@@ -6789,7 +6893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:E14"/>
     </sheetView>
   </sheetViews>
@@ -6823,14 +6927,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="172"/>
+      <c r="M2" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="172"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -6861,14 +6965,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="170" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="171"/>
+      <c r="C4" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="174"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -6895,10 +6999,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -6914,10 +7018,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="170" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -6930,10 +7034,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -6943,10 +7047,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -6956,10 +7060,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="170" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -6969,10 +7073,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -6982,10 +7086,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -6996,8 +7100,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7009,13 +7113,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -7057,12 +7161,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7070,6 +7168,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7083,7 +7187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:O17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:E14"/>
     </sheetView>
   </sheetViews>
@@ -7116,14 +7220,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="172"/>
+      <c r="M2" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="172"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7154,14 +7258,14 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="170" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="171"/>
+      <c r="C4" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="174"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7188,10 +7292,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="170" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7207,10 +7311,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="170" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7223,10 +7327,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7236,10 +7340,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7249,10 +7353,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="170" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7262,10 +7366,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7275,10 +7379,10 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7290,8 +7394,8 @@
       <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7303,13 +7407,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -7351,12 +7455,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7364,6 +7462,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7410,14 +7514,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="172"/>
+      <c r="M2" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="172"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7448,12 +7552,12 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="170"/>
+      <c r="B4" s="171"/>
+      <c r="C4" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="174"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7480,10 +7584,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="170" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7499,10 +7603,10 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="170" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7515,10 +7619,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="170" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7528,10 +7632,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="170" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7541,10 +7645,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="170" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7554,10 +7658,10 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7567,10 +7671,10 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7582,8 +7686,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7599,13 +7703,13 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
@@ -7647,12 +7751,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7660,6 +7758,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7708,14 +7812,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="172"/>
+      <c r="M2" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="172"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7746,14 +7850,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="170" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="171"/>
+      <c r="C4" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="174"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7780,10 +7884,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7799,10 +7903,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="170" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7815,10 +7919,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="170" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7828,10 +7932,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7841,10 +7945,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7854,10 +7958,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="170" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7867,10 +7971,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7881,10 +7985,10 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176" t="s">
+      <c r="A12" s="170" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="177"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7897,13 +8001,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -7945,12 +8049,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7958,6 +8056,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165359" right="0.41338582677165359" top="0.41338582677165359" bottom="0.41338582677165359" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8005,14 +8109,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="172"/>
+      <c r="M2" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="172"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -8043,12 +8147,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="170"/>
+      <c r="B4" s="171"/>
+      <c r="C4" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="174"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8075,10 +8179,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="170" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8094,10 +8198,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8110,10 +8214,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="170" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8125,10 +8229,10 @@
       <c r="O7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8139,10 +8243,10 @@
       <c r="E8" s="49"/>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="170" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8152,10 +8256,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="170" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8165,8 +8269,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="170"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8178,8 +8282,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8193,13 +8297,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -8241,12 +8345,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8254,6 +8352,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8300,14 +8404,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="172"/>
+      <c r="M2" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="172"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -8338,12 +8442,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="170"/>
+      <c r="B4" s="171"/>
+      <c r="C4" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="174"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8370,8 +8474,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="170"/>
+      <c r="B5" s="171"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8387,10 +8491,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="170" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="171"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8403,10 +8507,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="171"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8416,10 +8520,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="170" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8429,10 +8533,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="170" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="171"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8442,8 +8546,8 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="170"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8453,8 +8557,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="170"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8466,8 +8570,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="170"/>
+      <c r="B12" s="171"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8480,13 +8584,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="175" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -8531,12 +8635,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8544,6 +8642,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixing bug missing on missing water usage.
</commit_message>
<xml_diff>
--- a/Bookkeeping.xlsx
+++ b/Bookkeeping.xlsx
@@ -356,19 +356,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="13">
-    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0\ \k\W&quot;h&quot;"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00\ \L\ "/>
-    <numFmt numFmtId="169" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="#,##0.00\ &quot;€&quot;&quot;/m²&quot;;\-#,##0.00\ &quot;€&quot;&quot;/m²&quot;"/>
-    <numFmt numFmtId="172" formatCode="#,##0.00\ &quot;€&quot;&quot;/m³&quot;;\-#,##0.00\ &quot;€&quot;&quot;/m³&quot;"/>
-    <numFmt numFmtId="173" formatCode="#,##0.00\ &quot;m&quot;\³"/>
-    <numFmt numFmtId="174" formatCode="#,##0.00\ &quot;m&quot;\²"/>
-    <numFmt numFmtId="175" formatCode="#,##0.000000\ \k\W&quot;h&quot;"/>
-    <numFmt numFmtId="176" formatCode="#,##0.000\ &quot;m&quot;\³"/>
+    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0\ \k\W&quot;h&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ \L\ "/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;€&quot;&quot;/m²&quot;;\-#,##0.00\ &quot;€&quot;&quot;/m²&quot;"/>
+    <numFmt numFmtId="169" formatCode="#,##0.00\ &quot;€&quot;&quot;/m³&quot;;\-#,##0.00\ &quot;€&quot;&quot;/m³&quot;"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00\ &quot;m&quot;\³"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00\ &quot;m&quot;\²"/>
+    <numFmt numFmtId="172" formatCode="#,##0.000000\ \k\W&quot;h&quot;"/>
+    <numFmt numFmtId="173" formatCode="#,##0.000\ &quot;m&quot;\³"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -789,7 +789,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -799,8 +799,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -818,49 +818,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="6" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -879,7 +879,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -887,7 +887,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -897,7 +897,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -916,14 +916,14 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -949,25 +949,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
@@ -989,19 +989,19 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1010,25 +1010,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
@@ -1044,13 +1044,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1068,8 +1068,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1095,17 +1095,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1177,6 +1177,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1184,21 +1199,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1892,24 +1892,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="73684864"/>
-        <c:axId val="73686400"/>
+        <c:axId val="92218880"/>
+        <c:axId val="92220416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73684864"/>
+        <c:axId val="92218880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73686400"/>
+        <c:crossAx val="92220416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73686400"/>
+        <c:axId val="92220416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1918,7 +1918,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73684864"/>
+        <c:crossAx val="92218880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1936,7 +1936,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001377" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001388" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001388" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2183,24 +2183,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="73785344"/>
-        <c:axId val="73786880"/>
+        <c:axId val="92573056"/>
+        <c:axId val="92583040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73785344"/>
+        <c:axId val="92573056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73786880"/>
+        <c:crossAx val="92583040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73786880"/>
+        <c:axId val="92583040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2208,19 +2208,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73785344"/>
+        <c:crossAx val="92573056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000799" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000799" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.7500000000000081" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000081" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2751,7 +2752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
@@ -3361,14 +3362,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3399,12 +3400,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3431,8 +3432,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3448,10 +3449,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3464,10 +3465,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3477,10 +3478,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3490,10 +3491,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3503,8 +3504,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="173"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3515,8 +3516,8 @@
       <c r="F10" s="49"/>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3527,8 +3528,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -3542,13 +3543,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -3590,12 +3591,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -3603,6 +3598,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3650,14 +3651,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3688,12 +3689,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3720,8 +3721,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3737,8 +3738,8 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176"/>
-      <c r="B6" s="177"/>
+      <c r="A6" s="173"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3751,10 +3752,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3765,10 +3766,10 @@
       <c r="E7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3778,10 +3779,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3791,8 +3792,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="173"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3802,8 +3803,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3815,8 +3816,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -3829,13 +3830,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -3877,12 +3878,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -3890,6 +3885,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3938,14 +3939,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3976,12 +3977,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4008,8 +4009,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4025,10 +4026,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4041,10 +4042,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4054,10 +4055,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4067,10 +4068,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4080,10 +4081,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4093,8 +4094,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4105,8 +4106,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4122,13 +4123,13 @@
       <c r="O13" s="49"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -4170,12 +4171,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4183,6 +4178,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4229,14 +4230,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4267,12 +4268,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4299,8 +4300,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4316,10 +4317,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4332,10 +4333,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4345,10 +4346,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4358,10 +4359,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4371,10 +4372,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4384,8 +4385,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4397,8 +4398,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4413,13 +4414,13 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="121" t="s">
@@ -4461,12 +4462,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4474,6 +4469,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4521,14 +4522,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4559,14 +4560,14 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="173" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4593,10 +4594,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4612,10 +4613,10 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4628,10 +4629,10 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4641,10 +4642,10 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4654,10 +4655,10 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4667,10 +4668,10 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4680,10 +4681,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4695,8 +4696,8 @@
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4710,13 +4711,13 @@
     </row>
     <row r="13" spans="1:16" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="121" t="s">
@@ -4758,12 +4759,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4771,6 +4766,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4817,14 +4818,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4855,12 +4856,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4887,10 +4888,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4905,10 +4906,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4920,10 +4921,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4933,10 +4934,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4946,10 +4947,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4959,10 +4960,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4972,10 +4973,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4986,8 +4987,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -5001,13 +5002,13 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="121" t="s">
@@ -5075,7 +5076,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5094,7 +5097,7 @@
     <row r="1" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:13">
       <c r="A2" s="154">
-        <v>2012</v>
+        <v>2016</v>
       </c>
       <c r="B2" s="155"/>
       <c r="C2" s="155"/>
@@ -5768,7 +5771,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:T32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -6822,7 +6827,7 @@
         <v>88</v>
       </c>
       <c r="M29" s="116">
-        <f>N22-N10</f>
+        <f>(N22-N10)+(M25)</f>
         <v>0</v>
       </c>
       <c r="N29" s="115">
@@ -6926,14 +6931,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -6964,14 +6969,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="173" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -6998,10 +7003,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7017,10 +7022,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7033,10 +7038,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7046,10 +7051,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7059,10 +7064,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7072,10 +7077,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7085,10 +7090,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7099,8 +7104,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7112,13 +7117,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -7160,12 +7165,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7173,6 +7172,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7219,14 +7224,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7257,14 +7262,14 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7291,10 +7296,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7310,10 +7315,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7326,10 +7331,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7339,10 +7344,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7352,10 +7357,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7365,10 +7370,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7378,10 +7383,10 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7393,8 +7398,8 @@
       <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7406,13 +7411,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -7454,12 +7459,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7467,6 +7466,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7513,14 +7518,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7551,12 +7556,12 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7583,10 +7588,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7602,10 +7607,10 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7618,10 +7623,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7631,10 +7636,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7644,10 +7649,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7657,10 +7662,10 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7670,10 +7675,10 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7685,8 +7690,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7702,13 +7707,13 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
@@ -7750,12 +7755,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7763,6 +7762,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7811,14 +7816,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7849,14 +7854,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7883,10 +7888,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7902,10 +7907,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7918,10 +7923,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7931,10 +7936,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7944,10 +7949,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7957,10 +7962,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7970,10 +7975,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7984,10 +7989,10 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176" t="s">
+      <c r="A12" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="177"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8000,13 +8005,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -8048,12 +8053,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8061,6 +8060,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165359" right="0.41338582677165359" top="0.41338582677165359" bottom="0.41338582677165359" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8108,14 +8113,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -8146,12 +8151,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8178,10 +8183,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8197,10 +8202,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8213,10 +8218,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8228,10 +8233,10 @@
       <c r="O7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8242,10 +8247,10 @@
       <c r="E8" s="49"/>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8255,10 +8260,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8268,8 +8273,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8281,8 +8286,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8296,13 +8301,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -8344,12 +8349,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8357,6 +8356,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8403,14 +8408,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -8441,12 +8446,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8473,8 +8478,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8490,10 +8495,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8506,10 +8511,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8519,10 +8524,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8532,10 +8537,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8545,8 +8550,8 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="173"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8556,8 +8561,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8569,8 +8574,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8583,13 +8588,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -8634,12 +8639,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8647,6 +8646,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating targets for 2015.
</commit_message>
<xml_diff>
--- a/Bookkeeping.xlsx
+++ b/Bookkeeping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="18735" windowHeight="8340" tabRatio="873" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="18735" windowHeight="8340" tabRatio="873"/>
   </bookViews>
   <sheets>
     <sheet name="Targets" sheetId="15" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Overview!$A$1:$H$39</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -1177,6 +1177,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1190,15 +1199,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1454,7 +1454,7 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="6"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
@@ -1463,6 +1463,69 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>2014</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Targets!$X$17:$X$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.34499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.105</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Targets!$Y$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2015</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1526,45 +1589,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Targets!$X$17:$X$28</c:f>
+              <c:f>Targets!$Y$17:$Y$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.38500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.15</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.42</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.34499999999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.23499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.4999999999999997E-2</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>-0.01</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.105</c:v>
+                  <c:v>-0.06</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>-0.245</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>4.4999999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1572,7 +1635,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Targets!$T$15</c:f>
@@ -1679,7 +1742,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Targets!$S$15</c:f>
@@ -1786,7 +1849,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="5"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>Targets!$U$15</c:f>
@@ -1892,24 +1955,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92218880"/>
-        <c:axId val="92220416"/>
+        <c:axId val="72370048"/>
+        <c:axId val="72371584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92218880"/>
+        <c:axId val="72370048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92220416"/>
+        <c:crossAx val="72371584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92220416"/>
+        <c:axId val="72371584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1918,7 +1981,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92218880"/>
+        <c:crossAx val="72370048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1936,7 +1999,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001388" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001388" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001399" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001399" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2183,24 +2246,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92573056"/>
-        <c:axId val="92583040"/>
+        <c:axId val="72400896"/>
+        <c:axId val="72402432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92573056"/>
+        <c:axId val="72400896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92583040"/>
+        <c:crossAx val="72402432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92583040"/>
+        <c:axId val="72402432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2208,20 +2271,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92573056"/>
+        <c:crossAx val="72400896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.7500000000000081" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000081" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000822" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000822" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2750,10 +2812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X28"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2763,7 +2825,7 @@
     <col min="16" max="18" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="150" t="s">
         <v>105</v>
       </c>
@@ -2781,27 +2843,27 @@
       <c r="M1" s="150"/>
       <c r="N1" s="150"/>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:25">
       <c r="P9" s="146"/>
       <c r="Q9" s="146"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:25">
       <c r="P10" s="146"/>
       <c r="Q10" s="146"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:25">
       <c r="P11" s="146"/>
       <c r="Q11" s="146"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:25">
       <c r="P12" s="146"/>
       <c r="Q12" s="146"/>
       <c r="R12" s="49"/>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:25">
       <c r="P15" s="138" t="s">
         <v>90</v>
       </c>
@@ -2829,8 +2891,11 @@
       <c r="X15">
         <v>2014</v>
       </c>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="Y15">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
       <c r="P16" s="3">
         <v>0</v>
       </c>
@@ -2859,8 +2924,11 @@
       <c r="X16" s="117">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="15:24">
+      <c r="Y16" s="117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="15:25">
       <c r="O17" s="137" t="s">
         <v>49</v>
       </c>
@@ -2896,8 +2964,11 @@
       <c r="X17" s="117">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="15:24">
+      <c r="Y17" s="117">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="18" spans="15:25">
       <c r="O18" s="137" t="s">
         <v>50</v>
       </c>
@@ -2934,8 +3005,11 @@
       <c r="X18" s="117">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="19" spans="15:24">
+      <c r="Y18" s="117">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="19" spans="15:25">
       <c r="O19" s="137" t="s">
         <v>51</v>
       </c>
@@ -2972,8 +3046,11 @@
       <c r="X19" s="117">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="20" spans="15:24">
+      <c r="Y19" s="117">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="20" spans="15:25">
       <c r="O20" s="137" t="s">
         <v>52</v>
       </c>
@@ -3010,8 +3087,11 @@
       <c r="X20" s="117">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="21" spans="15:24">
+      <c r="Y20" s="117">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="21" spans="15:25">
       <c r="O21" s="137" t="s">
         <v>53</v>
       </c>
@@ -3048,8 +3128,11 @@
       <c r="X21" s="117">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="22" spans="15:24">
+      <c r="Y21" s="117">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="22" spans="15:25">
       <c r="O22" s="137" t="s">
         <v>54</v>
       </c>
@@ -3086,8 +3169,11 @@
       <c r="X22" s="117">
         <v>0.34499999999999997</v>
       </c>
-    </row>
-    <row r="23" spans="15:24">
+      <c r="Y22" s="117">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="15:25">
       <c r="O23" s="137" t="s">
         <v>55</v>
       </c>
@@ -3124,8 +3210,11 @@
       <c r="X23" s="117">
         <v>0.23499999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="15:24">
+      <c r="Y23" s="117">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="15:25">
       <c r="O24" s="137" t="s">
         <v>56</v>
       </c>
@@ -3162,8 +3251,11 @@
       <c r="X24" s="117">
         <v>7.4999999999999997E-2</v>
       </c>
-    </row>
-    <row r="25" spans="15:24">
+      <c r="Y24" s="117">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="25" spans="15:25">
       <c r="O25" s="137" t="s">
         <v>57</v>
       </c>
@@ -3200,8 +3292,11 @@
       <c r="X25" s="117">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="15:24">
+      <c r="Y25" s="117">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="15:25">
       <c r="O26" s="137" t="s">
         <v>58</v>
       </c>
@@ -3238,8 +3333,11 @@
       <c r="X26" s="117">
         <v>-0.105</v>
       </c>
-    </row>
-    <row r="27" spans="15:24">
+      <c r="Y26" s="117">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="27" spans="15:25">
       <c r="O27" s="137" t="s">
         <v>59</v>
       </c>
@@ -3276,8 +3374,11 @@
       <c r="X27" s="117">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="15:24">
+      <c r="Y27" s="117">
+        <v>-0.245</v>
+      </c>
+    </row>
+    <row r="28" spans="15:25">
       <c r="O28" s="137" t="s">
         <v>60</v>
       </c>
@@ -3312,6 +3413,9 @@
       </c>
       <c r="X28" s="117">
         <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y28" s="117">
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3362,14 +3466,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3400,12 +3504,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3432,8 +3536,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="173"/>
-      <c r="B5" s="174"/>
+      <c r="A5" s="176"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3449,10 +3553,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3465,10 +3569,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3478,10 +3582,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3491,10 +3595,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3504,8 +3608,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="173"/>
-      <c r="B10" s="174"/>
+      <c r="A10" s="176"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3516,8 +3620,8 @@
       <c r="F10" s="49"/>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3528,8 +3632,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -3543,13 +3647,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -3591,6 +3695,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -3598,12 +3708,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3651,14 +3755,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3689,12 +3793,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3721,8 +3825,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="173"/>
-      <c r="B5" s="174"/>
+      <c r="A5" s="176"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3738,8 +3842,8 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="173"/>
-      <c r="B6" s="174"/>
+      <c r="A6" s="176"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3752,10 +3856,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3766,10 +3870,10 @@
       <c r="E7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3779,10 +3883,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3792,8 +3896,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="173"/>
-      <c r="B10" s="174"/>
+      <c r="A10" s="176"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3803,8 +3907,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3816,8 +3920,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -3830,13 +3934,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -3878,6 +3982,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -3885,12 +3995,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3939,14 +4043,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3977,12 +4081,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4009,8 +4113,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="173"/>
-      <c r="B5" s="174"/>
+      <c r="A5" s="176"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4026,10 +4130,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4042,10 +4146,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4055,10 +4159,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4068,10 +4172,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4081,10 +4185,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4094,8 +4198,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4106,8 +4210,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4123,13 +4227,13 @@
       <c r="O13" s="49"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -4171,6 +4275,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4178,12 +4288,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4230,14 +4334,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4268,12 +4372,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4300,8 +4404,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="173"/>
-      <c r="B5" s="174"/>
+      <c r="A5" s="176"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4317,10 +4421,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4333,10 +4437,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4346,10 +4450,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4359,10 +4463,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4372,10 +4476,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4385,8 +4489,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4398,8 +4502,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4414,13 +4518,13 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="121" t="s">
@@ -4462,6 +4566,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4469,12 +4579,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4522,14 +4626,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4560,14 +4664,14 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A4" s="173" t="s">
+      <c r="A4" s="176" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4594,10 +4698,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4613,10 +4717,10 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4629,10 +4733,10 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4642,10 +4746,10 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4655,10 +4759,10 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4668,10 +4772,10 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4681,10 +4785,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4696,8 +4800,8 @@
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4711,13 +4815,13 @@
     </row>
     <row r="13" spans="1:16" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="121" t="s">
@@ -4759,6 +4863,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4766,12 +4876,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4818,14 +4922,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4856,12 +4960,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4888,10 +4992,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4906,10 +5010,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4921,10 +5025,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4934,10 +5038,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4947,10 +5051,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4960,10 +5064,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4973,10 +5077,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4987,8 +5091,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -5002,13 +5106,13 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="121" t="s">
@@ -5771,7 +5875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:T32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
@@ -6931,14 +7035,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -6969,14 +7073,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="173" t="s">
+      <c r="A4" s="176" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7003,10 +7107,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7022,10 +7126,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7038,10 +7142,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7051,10 +7155,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7064,10 +7168,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7077,10 +7181,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7090,10 +7194,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7104,8 +7208,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7117,13 +7221,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -7165,6 +7269,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7172,12 +7282,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7224,14 +7328,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7262,14 +7366,14 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="173" t="s">
+      <c r="A4" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7296,10 +7400,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7315,10 +7419,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7331,10 +7435,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7344,10 +7448,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7357,10 +7461,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7370,10 +7474,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7383,10 +7487,10 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7398,8 +7502,8 @@
       <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7411,13 +7515,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -7459,6 +7563,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7466,12 +7576,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7518,14 +7622,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7556,12 +7660,12 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7588,10 +7692,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7607,10 +7711,10 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7623,10 +7727,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7636,10 +7740,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7649,10 +7753,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7662,10 +7766,10 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7675,10 +7779,10 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7690,8 +7794,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7707,13 +7811,13 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
@@ -7755,6 +7859,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7762,12 +7872,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7816,14 +7920,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7854,14 +7958,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="173" t="s">
+      <c r="A4" s="176" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7888,10 +7992,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7907,10 +8011,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7923,10 +8027,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7936,10 +8040,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7949,10 +8053,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7962,10 +8066,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7975,10 +8079,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7989,10 +8093,10 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="173" t="s">
+      <c r="A12" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="174"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8005,13 +8109,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -8053,6 +8157,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8060,12 +8170,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165359" right="0.41338582677165359" top="0.41338582677165359" bottom="0.41338582677165359" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8113,14 +8217,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -8151,12 +8255,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8183,10 +8287,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8202,10 +8306,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8218,10 +8322,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8233,10 +8337,10 @@
       <c r="O7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8247,10 +8351,10 @@
       <c r="E8" s="49"/>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8260,10 +8364,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8273,8 +8377,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8286,8 +8390,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8301,13 +8405,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -8349,6 +8453,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8356,12 +8466,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8408,14 +8512,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -8446,12 +8550,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8478,8 +8582,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="173"/>
-      <c r="B5" s="174"/>
+      <c r="A5" s="176"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8495,10 +8599,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8511,10 +8615,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8524,10 +8628,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8537,10 +8641,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8550,8 +8654,8 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="173"/>
-      <c r="B10" s="174"/>
+      <c r="A10" s="176"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8561,8 +8665,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8574,8 +8678,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8588,13 +8692,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -8639,6 +8743,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8646,12 +8756,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reading savings data from data tables.
</commit_message>
<xml_diff>
--- a/Bookkeeping.xlsx
+++ b/Bookkeeping.xlsx
@@ -1177,6 +1177,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1184,21 +1199,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1955,24 +1955,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="72370048"/>
-        <c:axId val="72371584"/>
+        <c:axId val="91105536"/>
+        <c:axId val="91123712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72370048"/>
+        <c:axId val="91105536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72371584"/>
+        <c:crossAx val="91123712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72371584"/>
+        <c:axId val="91123712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1981,7 +1981,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72370048"/>
+        <c:crossAx val="91105536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1999,7 +1999,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001399" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001399" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.7500000000000141" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000141" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2246,24 +2246,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="72400896"/>
-        <c:axId val="72402432"/>
+        <c:axId val="91591040"/>
+        <c:axId val="91592576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72400896"/>
+        <c:axId val="91591040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72402432"/>
+        <c:crossAx val="91592576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72402432"/>
+        <c:axId val="91592576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2271,7 +2271,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72400896"/>
+        <c:crossAx val="91591040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2284,7 +2284,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000822" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000822" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000833" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000833" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2815,8 +2815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3475,14 +3475,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3513,12 +3513,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3545,8 +3545,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3562,10 +3562,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3578,10 +3578,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3591,10 +3591,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3604,10 +3604,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3617,8 +3617,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="173"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3629,8 +3629,8 @@
       <c r="F10" s="49"/>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3641,8 +3641,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -3656,13 +3656,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -3704,12 +3704,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -3717,6 +3711,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3764,14 +3764,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3802,12 +3802,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3834,8 +3834,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3851,8 +3851,8 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176"/>
-      <c r="B6" s="177"/>
+      <c r="A6" s="173"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3865,10 +3865,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3879,10 +3879,10 @@
       <c r="E7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3892,10 +3892,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3905,8 +3905,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="173"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3916,8 +3916,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3929,8 +3929,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -3943,13 +3943,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -3991,12 +3991,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4004,6 +3998,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4052,14 +4052,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4090,12 +4090,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4122,8 +4122,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4139,10 +4139,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4155,10 +4155,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4168,10 +4168,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4181,10 +4181,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4194,10 +4194,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4207,8 +4207,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4219,8 +4219,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4236,13 +4236,13 @@
       <c r="O13" s="49"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -4284,12 +4284,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4297,6 +4291,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4343,14 +4343,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4381,12 +4381,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4413,8 +4413,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4430,10 +4430,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4446,10 +4446,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4459,10 +4459,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4472,10 +4472,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4485,10 +4485,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4498,8 +4498,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4511,8 +4511,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4527,13 +4527,13 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="121" t="s">
@@ -4575,12 +4575,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4588,6 +4582,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4635,14 +4635,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4673,14 +4673,14 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="173" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4707,10 +4707,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4726,10 +4726,10 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4742,10 +4742,10 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4755,10 +4755,10 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4768,10 +4768,10 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4781,10 +4781,10 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4794,10 +4794,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4809,8 +4809,8 @@
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4824,13 +4824,13 @@
     </row>
     <row r="13" spans="1:16" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="121" t="s">
@@ -4872,12 +4872,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4885,6 +4879,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4931,14 +4931,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4969,12 +4969,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -5001,10 +5001,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -5019,10 +5019,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -5034,10 +5034,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -5047,10 +5047,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -5060,10 +5060,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -5073,10 +5073,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -5086,10 +5086,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -5100,8 +5100,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -5115,13 +5115,13 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="121" t="s">
@@ -5884,7 +5884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:T32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
@@ -7044,14 +7044,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7082,14 +7082,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="173" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7116,10 +7116,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7135,10 +7135,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7151,10 +7151,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7164,10 +7164,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7177,10 +7177,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7190,10 +7190,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7203,10 +7203,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7217,8 +7217,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7230,13 +7230,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -7278,12 +7278,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7291,6 +7285,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7337,14 +7337,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7375,14 +7375,14 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7409,10 +7409,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7428,10 +7428,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7444,10 +7444,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7457,10 +7457,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7470,10 +7470,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7483,10 +7483,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7496,10 +7496,10 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7511,8 +7511,8 @@
       <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7524,13 +7524,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -7572,12 +7572,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7585,6 +7579,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7631,14 +7631,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7669,12 +7669,12 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7701,10 +7701,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7720,10 +7720,10 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7736,10 +7736,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7749,10 +7749,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7762,10 +7762,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7775,10 +7775,10 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7788,10 +7788,10 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7803,8 +7803,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7820,13 +7820,13 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
@@ -7868,12 +7868,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7881,6 +7875,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7929,14 +7929,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7967,14 +7967,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8001,10 +8001,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8020,10 +8020,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8036,10 +8036,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8049,10 +8049,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8062,10 +8062,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8075,10 +8075,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8088,10 +8088,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8102,10 +8102,10 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176" t="s">
+      <c r="A12" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="177"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8118,13 +8118,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -8166,12 +8166,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8179,6 +8173,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165359" right="0.41338582677165359" top="0.41338582677165359" bottom="0.41338582677165359" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8226,14 +8226,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -8264,12 +8264,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8296,10 +8296,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8315,10 +8315,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8331,10 +8331,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8346,10 +8346,10 @@
       <c r="O7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8360,10 +8360,10 @@
       <c r="E8" s="49"/>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8373,10 +8373,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8386,8 +8386,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8399,8 +8399,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8414,13 +8414,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -8462,12 +8462,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8475,6 +8469,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8521,14 +8521,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -8559,12 +8559,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8591,8 +8591,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8608,10 +8608,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8624,10 +8624,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8637,10 +8637,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8650,10 +8650,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8663,8 +8663,8 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="173"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8674,8 +8674,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8687,8 +8687,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8701,13 +8701,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -8752,12 +8752,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8765,6 +8759,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixing bug in Targets.
</commit_message>
<xml_diff>
--- a/Bookkeeping.xlsx
+++ b/Bookkeeping.xlsx
@@ -1177,6 +1177,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1190,15 +1199,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1406,47 +1406,44 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Targets!$W$16:$W$28</c:f>
+              <c:f>Targets!$W$17:$W$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.7619047619047624E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.7619047619047624E-2</c:v>
+                  <c:v>0.17523809523809525</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17523809523809525</c:v>
+                  <c:v>0.21333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.21333333333333335</c:v>
+                  <c:v>0.28190476190476188</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.28190476190476188</c:v>
+                  <c:v>0.37333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.37333333333333335</c:v>
+                  <c:v>0.45714285714285713</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45714285714285713</c:v>
+                  <c:v>0.70095238095238099</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.70095238095238099</c:v>
+                  <c:v>0.78476190476190477</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.78476190476190477</c:v>
+                  <c:v>0.86857142857142855</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.86857142857142855</c:v>
+                  <c:v>0.95238095238095233</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.95238095238095233</c:v>
+                  <c:v>1.0361904761904761</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0361904761904761</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>1.1200000000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -1955,24 +1952,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="91105536"/>
-        <c:axId val="91123712"/>
+        <c:axId val="121782656"/>
+        <c:axId val="121784192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91105536"/>
+        <c:axId val="121782656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91123712"/>
+        <c:crossAx val="121784192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91123712"/>
+        <c:axId val="121784192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1981,7 +1978,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91105536"/>
+        <c:crossAx val="121782656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1999,7 +1996,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.7500000000000141" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000141" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001421" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001421" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2246,24 +2243,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="91591040"/>
-        <c:axId val="91592576"/>
+        <c:axId val="126204160"/>
+        <c:axId val="126259200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91591040"/>
+        <c:axId val="126204160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91592576"/>
+        <c:crossAx val="126259200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91592576"/>
+        <c:axId val="126259200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2271,20 +2268,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91591040"/>
+        <c:crossAx val="126204160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000833" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000833" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000844" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000844" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2815,7 +2811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -3475,14 +3471,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3513,12 +3509,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3545,8 +3541,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="173"/>
-      <c r="B5" s="174"/>
+      <c r="A5" s="176"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3562,10 +3558,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3578,10 +3574,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3591,10 +3587,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3604,10 +3600,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3617,8 +3613,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="173"/>
-      <c r="B10" s="174"/>
+      <c r="A10" s="176"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3629,8 +3625,8 @@
       <c r="F10" s="49"/>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3641,8 +3637,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -3656,13 +3652,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -3704,6 +3700,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -3711,12 +3713,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3764,14 +3760,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3802,12 +3798,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3834,8 +3830,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="173"/>
-      <c r="B5" s="174"/>
+      <c r="A5" s="176"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3851,8 +3847,8 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="173"/>
-      <c r="B6" s="174"/>
+      <c r="A6" s="176"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3865,10 +3861,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3879,10 +3875,10 @@
       <c r="E7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3892,10 +3888,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3905,8 +3901,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="173"/>
-      <c r="B10" s="174"/>
+      <c r="A10" s="176"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3916,8 +3912,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3929,8 +3925,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -3943,13 +3939,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -3991,6 +3987,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -3998,12 +4000,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4052,14 +4048,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4090,12 +4086,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4122,8 +4118,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="173"/>
-      <c r="B5" s="174"/>
+      <c r="A5" s="176"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4139,10 +4135,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4155,10 +4151,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4168,10 +4164,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4181,10 +4177,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4194,10 +4190,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4207,8 +4203,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4219,8 +4215,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4236,13 +4232,13 @@
       <c r="O13" s="49"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -4284,6 +4280,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4291,12 +4293,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4343,14 +4339,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4381,12 +4377,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4413,8 +4409,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="173"/>
-      <c r="B5" s="174"/>
+      <c r="A5" s="176"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4430,10 +4426,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4446,10 +4442,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4459,10 +4455,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4472,10 +4468,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4485,10 +4481,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4498,8 +4494,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4511,8 +4507,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4527,13 +4523,13 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="121" t="s">
@@ -4575,6 +4571,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4582,12 +4584,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4635,14 +4631,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4673,14 +4669,14 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A4" s="173" t="s">
+      <c r="A4" s="176" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4707,10 +4703,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4726,10 +4722,10 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4742,10 +4738,10 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4755,10 +4751,10 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4768,10 +4764,10 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4781,10 +4777,10 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4794,10 +4790,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4809,8 +4805,8 @@
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4824,13 +4820,13 @@
     </row>
     <row r="13" spans="1:16" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="121" t="s">
@@ -4872,6 +4868,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4879,12 +4881,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4931,14 +4927,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4969,12 +4965,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -5001,10 +4997,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -5019,10 +5015,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -5034,10 +5030,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -5047,10 +5043,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -5060,10 +5056,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -5073,10 +5069,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -5086,10 +5082,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -5100,8 +5096,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -5115,13 +5111,13 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="121" t="s">
@@ -7044,14 +7040,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7082,14 +7078,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="173" t="s">
+      <c r="A4" s="176" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7116,10 +7112,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7135,10 +7131,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7151,10 +7147,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7164,10 +7160,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7177,10 +7173,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7190,10 +7186,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7203,10 +7199,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7217,8 +7213,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7230,13 +7226,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -7278,6 +7274,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7285,12 +7287,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7337,14 +7333,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7375,14 +7371,14 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="173" t="s">
+      <c r="A4" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7409,10 +7405,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7428,10 +7424,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7444,10 +7440,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7457,10 +7453,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7470,10 +7466,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7483,10 +7479,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7496,10 +7492,10 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7511,8 +7507,8 @@
       <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7524,13 +7520,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -7572,6 +7568,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7579,12 +7581,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7631,14 +7627,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7669,12 +7665,12 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7701,10 +7697,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7720,10 +7716,10 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7736,10 +7732,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7749,10 +7745,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7762,10 +7758,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7775,10 +7771,10 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7788,10 +7784,10 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7803,8 +7799,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7820,13 +7816,13 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
@@ -7868,6 +7864,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7875,12 +7877,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7929,14 +7925,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7967,14 +7963,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="173" t="s">
+      <c r="A4" s="176" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8001,10 +7997,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8020,10 +8016,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8036,10 +8032,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8049,10 +8045,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8062,10 +8058,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8075,10 +8071,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8088,10 +8084,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="176" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8102,10 +8098,10 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="173" t="s">
+      <c r="A12" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="174"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8118,13 +8114,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -8166,6 +8162,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8173,12 +8175,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165359" right="0.41338582677165359" top="0.41338582677165359" bottom="0.41338582677165359" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8226,14 +8222,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -8264,12 +8260,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8296,10 +8292,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="174"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8315,10 +8311,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8331,10 +8327,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8346,10 +8342,10 @@
       <c r="O7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8360,10 +8356,10 @@
       <c r="E8" s="49"/>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8373,10 +8369,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="173" t="s">
+      <c r="A10" s="176" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="174"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8386,8 +8382,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8399,8 +8395,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8414,13 +8410,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -8462,6 +8458,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8469,12 +8471,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8521,14 +8517,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175" t="s">
+      <c r="L2" s="178"/>
+      <c r="M2" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="175"/>
+      <c r="N2" s="178"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -8559,12 +8555,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="173"/>
-      <c r="B4" s="174"/>
-      <c r="C4" s="176" t="s">
+      <c r="A4" s="176"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="177"/>
+      <c r="D4" s="180"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8591,8 +8587,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="173"/>
-      <c r="B5" s="174"/>
+      <c r="A5" s="176"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8608,10 +8604,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="173" t="s">
+      <c r="A6" s="176" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="174"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8624,10 +8620,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="174"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8637,10 +8633,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="176" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="174"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8650,10 +8646,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="173" t="s">
+      <c r="A9" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="174"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8663,8 +8659,8 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="173"/>
-      <c r="B10" s="174"/>
+      <c r="A10" s="176"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8674,8 +8670,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="173"/>
-      <c r="B11" s="174"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8687,8 +8683,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="173"/>
-      <c r="B12" s="174"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8701,13 +8697,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="178" t="s">
+      <c r="A14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="180"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -8752,6 +8748,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8759,12 +8761,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating targets with 2016.
</commit_message>
<xml_diff>
--- a/Bookkeeping.xlsx
+++ b/Bookkeeping.xlsx
@@ -348,7 +348,7 @@
     <t>Financial Transactions</t>
   </si>
   <si>
-    <t>Financial Targets for 2014</t>
+    <t>Financial Targets for 2017</t>
   </si>
 </sst>
 </file>
@@ -1177,6 +1177,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1184,21 +1199,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1631,8 +1631,71 @@
           </c:val>
         </c:ser>
         <c:ser>
+          <c:idx val="7"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Targets!$Z$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Targets!$Z$17:$Z$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.183</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.27300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28949999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33450000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.54949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.59950000000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.76449999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="4"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Targets!$T$15</c:f>
@@ -1739,7 +1802,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="5"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
               <c:f>Targets!$S$15</c:f>
@@ -1846,7 +1909,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="6"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
               <c:f>Targets!$U$15</c:f>
@@ -1952,24 +2015,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="121782656"/>
-        <c:axId val="121784192"/>
+        <c:axId val="39276928"/>
+        <c:axId val="39278464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121782656"/>
+        <c:axId val="39276928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121784192"/>
+        <c:crossAx val="39278464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121784192"/>
+        <c:axId val="39278464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1978,7 +2041,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121782656"/>
+        <c:crossAx val="39276928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1996,7 +2059,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001421" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001421" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001432" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001432" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2243,24 +2306,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="126204160"/>
-        <c:axId val="126259200"/>
+        <c:axId val="39672064"/>
+        <c:axId val="39677952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126204160"/>
+        <c:axId val="39672064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126259200"/>
+        <c:crossAx val="39677952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126259200"/>
+        <c:axId val="39677952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2268,19 +2331,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126204160"/>
+        <c:crossAx val="39672064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000844" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000844" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000855" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000855" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2811,8 +2875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2898,6 +2962,9 @@
       <c r="Y15">
         <v>2015</v>
       </c>
+      <c r="Z15">
+        <v>2016</v>
+      </c>
     </row>
     <row r="16" spans="1:27">
       <c r="P16" s="3">
@@ -2931,8 +2998,11 @@
       <c r="Y16" s="117">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="15:25">
+      <c r="Z16" s="117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="15:26">
       <c r="O17" s="137" t="s">
         <v>49</v>
       </c>
@@ -2972,8 +3042,11 @@
       <c r="Y17" s="117">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="18" spans="15:25">
+      <c r="Z17" s="117">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="15:26">
       <c r="O18" s="137" t="s">
         <v>50</v>
       </c>
@@ -3013,8 +3086,11 @@
       <c r="Y18" s="117">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="19" spans="15:25">
+      <c r="Z18" s="117">
+        <v>-5.5E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="15:26">
       <c r="O19" s="137" t="s">
         <v>51</v>
       </c>
@@ -3054,8 +3130,11 @@
       <c r="Y19" s="117">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="20" spans="15:25">
+      <c r="Z19" s="117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="15:26">
       <c r="O20" s="137" t="s">
         <v>52</v>
       </c>
@@ -3095,8 +3174,11 @@
       <c r="Y20" s="117">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="21" spans="15:25">
+      <c r="Z20" s="117">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="15:26">
       <c r="O21" s="137" t="s">
         <v>53</v>
       </c>
@@ -3136,8 +3218,11 @@
       <c r="Y21" s="117">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="22" spans="15:25">
+      <c r="Z21" s="117">
+        <v>0.183</v>
+      </c>
+    </row>
+    <row r="22" spans="15:26">
       <c r="O22" s="137" t="s">
         <v>54</v>
       </c>
@@ -3177,8 +3262,11 @@
       <c r="Y22" s="117">
         <v>0.38500000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="15:25">
+      <c r="Z22" s="117">
+        <v>0.27300000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="15:26">
       <c r="O23" s="137" t="s">
         <v>55</v>
       </c>
@@ -3218,8 +3306,11 @@
       <c r="Y23" s="117">
         <v>0.22500000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="15:25">
+      <c r="Z23" s="117">
+        <v>0.24299999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="15:26">
       <c r="O24" s="137" t="s">
         <v>56</v>
       </c>
@@ -3259,8 +3350,11 @@
       <c r="Y24" s="117">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="25" spans="15:25">
+      <c r="Z24" s="117">
+        <v>0.28949999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="15:26">
       <c r="O25" s="137" t="s">
         <v>57</v>
       </c>
@@ -3300,8 +3394,11 @@
       <c r="Y25" s="117">
         <v>-0.01</v>
       </c>
-    </row>
-    <row r="26" spans="15:25">
+      <c r="Z25" s="117">
+        <v>0.33450000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="15:26">
       <c r="O26" s="137" t="s">
         <v>58</v>
       </c>
@@ -3341,8 +3438,11 @@
       <c r="Y26" s="117">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="27" spans="15:25">
+      <c r="Z26" s="117">
+        <v>0.54949999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="15:26">
       <c r="O27" s="137" t="s">
         <v>59</v>
       </c>
@@ -3382,8 +3482,11 @@
       <c r="Y27" s="117">
         <v>-0.245</v>
       </c>
-    </row>
-    <row r="28" spans="15:25">
+      <c r="Z27" s="117">
+        <v>0.59950000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="15:26">
       <c r="O28" s="137" t="s">
         <v>60</v>
       </c>
@@ -3421,6 +3524,9 @@
       </c>
       <c r="Y28" s="117">
         <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="Z28" s="117">
+        <v>0.76449999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -3471,14 +3577,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3509,12 +3615,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3541,8 +3647,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3558,10 +3664,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3574,10 +3680,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3587,10 +3693,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3600,10 +3706,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3613,8 +3719,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="173"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3625,8 +3731,8 @@
       <c r="F10" s="49"/>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3637,8 +3743,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -3652,13 +3758,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -3700,12 +3806,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -3713,6 +3813,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3760,14 +3866,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -3798,12 +3904,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -3830,8 +3936,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -3847,8 +3953,8 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176"/>
-      <c r="B6" s="177"/>
+      <c r="A6" s="173"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -3861,10 +3967,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -3875,10 +3981,10 @@
       <c r="E7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -3888,10 +3994,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3901,8 +4007,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="173"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -3912,8 +4018,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3925,8 +4031,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -3939,13 +4045,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -3987,12 +4093,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4000,6 +4100,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4048,14 +4154,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4086,12 +4192,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4118,8 +4224,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4135,10 +4241,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4151,10 +4257,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4164,10 +4270,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4177,10 +4283,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4190,10 +4296,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4203,8 +4309,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4215,8 +4321,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4232,13 +4338,13 @@
       <c r="O13" s="49"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="121" t="s">
@@ -4280,12 +4386,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4293,6 +4393,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4339,14 +4445,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4377,12 +4483,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4409,8 +4515,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4426,10 +4532,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4442,10 +4548,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4455,10 +4561,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4468,10 +4574,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4481,10 +4587,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4494,8 +4600,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4507,8 +4613,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4523,13 +4629,13 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="121" t="s">
@@ -4571,12 +4677,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4584,6 +4684,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4631,14 +4737,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4669,14 +4775,14 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="173" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4703,10 +4809,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -4722,10 +4828,10 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4738,10 +4844,10 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -4751,10 +4857,10 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4764,10 +4870,10 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -4777,10 +4883,10 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -4790,10 +4896,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4805,8 +4911,8 @@
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -4820,13 +4926,13 @@
     </row>
     <row r="13" spans="1:16" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:16" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="121" t="s">
@@ -4868,12 +4974,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -4881,6 +4981,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4927,14 +5033,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="120"/>
@@ -4965,12 +5071,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -4997,10 +5103,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -5015,10 +5121,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -5030,10 +5136,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -5043,10 +5149,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -5056,10 +5162,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -5069,10 +5175,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -5082,10 +5188,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -5096,8 +5202,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -5111,13 +5217,13 @@
       <c r="F13" s="49"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="121" t="s">
@@ -7040,14 +7146,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7078,14 +7184,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="173" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7112,10 +7218,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7131,10 +7237,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7147,10 +7253,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7160,10 +7266,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7173,10 +7279,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7186,10 +7292,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7199,10 +7305,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7213,8 +7319,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7226,13 +7332,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -7274,12 +7380,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7287,6 +7387,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7333,14 +7439,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7371,14 +7477,14 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7405,10 +7511,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7424,10 +7530,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7440,10 +7546,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7453,10 +7559,10 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7466,10 +7572,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7479,10 +7585,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7492,10 +7598,10 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7507,8 +7613,8 @@
       <c r="O11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7520,13 +7626,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -7568,12 +7674,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7581,6 +7681,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7627,14 +7733,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7665,12 +7771,12 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7697,10 +7803,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -7716,10 +7822,10 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -7732,10 +7838,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -7745,10 +7851,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -7758,10 +7864,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -7771,10 +7877,10 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -7784,10 +7890,10 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -7799,8 +7905,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:17" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -7816,13 +7922,13 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
@@ -7864,12 +7970,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -7877,6 +7977,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7925,14 +8031,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -7963,14 +8069,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -7997,10 +8103,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8016,10 +8122,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8032,10 +8138,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8045,10 +8151,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8058,10 +8164,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8071,10 +8177,10 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8084,10 +8190,10 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8098,10 +8204,10 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176" t="s">
+      <c r="A12" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="177"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8114,13 +8220,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -8162,12 +8268,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8175,6 +8275,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165359" right="0.41338582677165359" top="0.41338582677165359" bottom="0.41338582677165359" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8222,14 +8328,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -8260,12 +8366,12 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8292,10 +8398,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="177"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8311,10 +8417,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8327,10 +8433,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8342,10 +8448,10 @@
       <c r="O7" s="49"/>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8356,10 +8462,10 @@
       <c r="E8" s="49"/>
     </row>
     <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8369,10 +8475,10 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="173" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="177"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8382,8 +8488,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8395,8 +8501,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8410,13 +8516,13 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -8458,12 +8564,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8471,6 +8571,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8517,14 +8623,14 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="178"/>
-      <c r="M2" s="178" t="s">
+      <c r="L2" s="175"/>
+      <c r="M2" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="178"/>
+      <c r="N2" s="175"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
       <c r="A3" s="13"/>
@@ -8555,12 +8661,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="179" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="177"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -8587,8 +8693,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="176"/>
-      <c r="B5" s="177"/>
+      <c r="A5" s="173"/>
+      <c r="B5" s="174"/>
       <c r="C5" s="6" t="s">
         <v>33</v>
       </c>
@@ -8604,10 +8710,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="177"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -8620,10 +8726,10 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="177"/>
+      <c r="B7" s="174"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
@@ -8633,10 +8739,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="173" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="177"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -8646,10 +8752,10 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75">
-      <c r="A9" s="176" t="s">
+      <c r="A9" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="177"/>
+      <c r="B9" s="174"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
@@ -8659,8 +8765,8 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="173"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
@@ -8670,8 +8776,8 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
@@ -8683,8 +8789,8 @@
       <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:14" ht="16.5" thickBot="1">
-      <c r="A12" s="176"/>
-      <c r="B12" s="177"/>
+      <c r="A12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="14" t="s">
         <v>32</v>
       </c>
@@ -8697,13 +8803,13 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A14" s="173" t="s">
+      <c r="A14" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="174"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="180"/>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
@@ -8748,12 +8854,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -8761,6 +8861,12 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.41338582677165353" right="0.41338582677165353" top="0.41338582677165353" bottom="0.41338582677165353" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating targets with 2017.
</commit_message>
<xml_diff>
--- a/Bookkeeping.xlsx
+++ b/Bookkeeping.xlsx
@@ -348,7 +348,7 @@
     <t>Financial Transactions</t>
   </si>
   <si>
-    <t>Financial Targets for 2017</t>
+    <t>Financial Targets for 2018</t>
   </si>
 </sst>
 </file>
@@ -1635,11 +1635,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Targets!$Z$15</c:f>
+              <c:f>Targets!$AA$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2016</c:v>
+                  <c:v>2017</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1649,45 +1649,30 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Targets!$Z$17:$Z$28</c:f>
+              <c:f>Targets!$AA$17:$AA$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>-0.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.5E-2</c:v>
+                  <c:v>5.5E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.7999999999999999E-2</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.183</c:v>
+                  <c:v>0.245</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.27300000000000002</c:v>
+                  <c:v>0.35499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.24299999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.28949999999999998</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.33450000000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.54949999999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.59950000000000003</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.76449999999999996</c:v>
+                  <c:v>0.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2015,24 +2000,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="39276928"/>
-        <c:axId val="39278464"/>
+        <c:axId val="73512064"/>
+        <c:axId val="73514368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39276928"/>
+        <c:axId val="73512064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39278464"/>
+        <c:crossAx val="73514368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39278464"/>
+        <c:axId val="73514368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2041,7 +2026,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39276928"/>
+        <c:crossAx val="73512064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2059,7 +2044,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001432" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001432" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001454" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001454" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2306,24 +2291,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="39672064"/>
-        <c:axId val="39677952"/>
+        <c:axId val="83528320"/>
+        <c:axId val="101188736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39672064"/>
+        <c:axId val="83528320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39677952"/>
+        <c:crossAx val="101188736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39677952"/>
+        <c:axId val="101188736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2331,7 +2316,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39672064"/>
+        <c:crossAx val="83528320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2344,7 +2329,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000855" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000855" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000877" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000877" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2873,10 +2858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA28"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2884,10 +2869,10 @@
     <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="0" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:28">
       <c r="A1" s="150" t="s">
         <v>105</v>
       </c>
@@ -2905,33 +2890,33 @@
       <c r="M1" s="150"/>
       <c r="N1" s="150"/>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:28">
       <c r="P9" s="146"/>
       <c r="Q9" s="146"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:28">
       <c r="P10" s="146"/>
       <c r="Q10" s="146"/>
       <c r="R10" s="3"/>
-      <c r="AA10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27">
+      <c r="AB10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28">
       <c r="P11" s="146"/>
       <c r="Q11" s="146"/>
       <c r="R11" s="3"/>
-      <c r="AA11" t="s">
+      <c r="AB11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:28">
       <c r="P12" s="146"/>
       <c r="Q12" s="146"/>
       <c r="R12" s="49"/>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:28">
       <c r="P15" s="138" t="s">
         <v>90</v>
       </c>
@@ -2965,8 +2950,11 @@
       <c r="Z15">
         <v>2016</v>
       </c>
-    </row>
-    <row r="16" spans="1:27">
+      <c r="AA15">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28">
       <c r="P16" s="3">
         <v>0</v>
       </c>
@@ -3001,8 +2989,11 @@
       <c r="Z16" s="117">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="15:26">
+      <c r="AA16" s="117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="15:27">
       <c r="O17" s="137" t="s">
         <v>49</v>
       </c>
@@ -3015,7 +3006,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="R17" s="3">
-        <f>0+DSUM(Table2[#All],"Value",$AA$10:$AA$11)</f>
+        <f>0+DSUM(Table2[#All],"Value",$AB$10:$AB$11)</f>
         <v>0</v>
       </c>
       <c r="S17" s="117">
@@ -3045,8 +3036,11 @@
       <c r="Z17" s="117">
         <v>1.4999999999999999E-2</v>
       </c>
-    </row>
-    <row r="18" spans="15:26">
+      <c r="AA17" s="117">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="15:27">
       <c r="O18" s="137" t="s">
         <v>50</v>
       </c>
@@ -3059,7 +3053,7 @@
         <v>0.125</v>
       </c>
       <c r="R18" s="3">
-        <f>R17+DSUM(Table22[#All],"Value",$AA$10:$AA$11)</f>
+        <f>R17+DSUM(Table22[#All],"Value",$AB$10:$AB$11)</f>
         <v>0</v>
       </c>
       <c r="S18" s="117">
@@ -3089,8 +3083,11 @@
       <c r="Z18" s="117">
         <v>-5.5E-2</v>
       </c>
-    </row>
-    <row r="19" spans="15:26">
+      <c r="AA18" s="117">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="15:27">
       <c r="O19" s="137" t="s">
         <v>51</v>
       </c>
@@ -3103,7 +3100,7 @@
         <v>0.1875</v>
       </c>
       <c r="R19" s="3">
-        <f>R18+DSUM(Table224[#All],"Value",$AA$10:$AA$11)</f>
+        <f>R18+DSUM(Table224[#All],"Value",$AB$10:$AB$11)</f>
         <v>0</v>
       </c>
       <c r="S19" s="117">
@@ -3133,8 +3130,11 @@
       <c r="Z19" s="117">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="15:26">
+      <c r="AA19" s="117">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="20" spans="15:27">
       <c r="O20" s="137" t="s">
         <v>52</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>0.25</v>
       </c>
       <c r="R20" s="3">
-        <f>R19+DSUM(Table2245[#All],"Value",$AA$10:$AA$11)</f>
+        <f>R19+DSUM(Table2245[#All],"Value",$AB$10:$AB$11)</f>
         <v>0</v>
       </c>
       <c r="S20" s="117">
@@ -3177,8 +3177,11 @@
       <c r="Z20" s="117">
         <v>3.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="21" spans="15:26">
+      <c r="AA20" s="117">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="21" spans="15:27">
       <c r="O21" s="137" t="s">
         <v>53</v>
       </c>
@@ -3191,7 +3194,7 @@
         <v>0.3125</v>
       </c>
       <c r="R21" s="3">
-        <f>R20+DSUM(Table22456[#All],"Value",$AA$10:$AA$11)</f>
+        <f>R20+DSUM(Table22456[#All],"Value",$AB$10:$AB$11)</f>
         <v>0</v>
       </c>
       <c r="S21" s="117">
@@ -3221,8 +3224,11 @@
       <c r="Z21" s="117">
         <v>0.183</v>
       </c>
-    </row>
-    <row r="22" spans="15:26">
+      <c r="AA21" s="117">
+        <v>0.245</v>
+      </c>
+    </row>
+    <row r="22" spans="15:27">
       <c r="O22" s="137" t="s">
         <v>54</v>
       </c>
@@ -3235,7 +3241,7 @@
         <v>0.375</v>
       </c>
       <c r="R22" s="3">
-        <f>R21+DSUM(Table224567[#All],"Value",$AA$10:$AA$11)</f>
+        <f>R21+DSUM(Table224567[#All],"Value",$AB$10:$AB$11)</f>
         <v>0</v>
       </c>
       <c r="S22" s="117">
@@ -3265,8 +3271,11 @@
       <c r="Z22" s="117">
         <v>0.27300000000000002</v>
       </c>
-    </row>
-    <row r="23" spans="15:26">
+      <c r="AA22" s="117">
+        <v>0.35499999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="15:27">
       <c r="O23" s="137" t="s">
         <v>55</v>
       </c>
@@ -3279,7 +3288,7 @@
         <v>0.4375</v>
       </c>
       <c r="R23" s="3">
-        <f>R22+DSUM(Table2245678[#All],"Value",$AA$10:$AA$11)</f>
+        <f>R22+DSUM(Table2245678[#All],"Value",$AB$10:$AB$11)</f>
         <v>0</v>
       </c>
       <c r="S23" s="117">
@@ -3309,8 +3318,11 @@
       <c r="Z23" s="117">
         <v>0.24299999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="15:26">
+      <c r="AA23" s="117">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="24" spans="15:27">
       <c r="O24" s="137" t="s">
         <v>56</v>
       </c>
@@ -3323,7 +3335,7 @@
         <v>0.5</v>
       </c>
       <c r="R24" s="3">
-        <f>R23+DSUM(Table22456789[#All],"Value",$AA$10:$AA$11)</f>
+        <f>R23+DSUM(Table22456789[#All],"Value",$AB$10:$AB$11)</f>
         <v>0</v>
       </c>
       <c r="S24" s="117">
@@ -3353,8 +3365,9 @@
       <c r="Z24" s="117">
         <v>0.28949999999999998</v>
       </c>
-    </row>
-    <row r="25" spans="15:26">
+      <c r="AA24" s="117"/>
+    </row>
+    <row r="25" spans="15:27">
       <c r="O25" s="137" t="s">
         <v>57</v>
       </c>
@@ -3367,7 +3380,7 @@
         <v>0.5625</v>
       </c>
       <c r="R25" s="3">
-        <f>R24+DSUM(Table2245678910[#All],"Value",$AA$10:$AA$11)</f>
+        <f>R24+DSUM(Table2245678910[#All],"Value",$AB$10:$AB$11)</f>
         <v>0</v>
       </c>
       <c r="S25" s="117">
@@ -3397,8 +3410,9 @@
       <c r="Z25" s="117">
         <v>0.33450000000000002</v>
       </c>
-    </row>
-    <row r="26" spans="15:26">
+      <c r="AA25" s="117"/>
+    </row>
+    <row r="26" spans="15:27">
       <c r="O26" s="137" t="s">
         <v>58</v>
       </c>
@@ -3411,7 +3425,7 @@
         <v>0.625</v>
       </c>
       <c r="R26" s="3">
-        <f>R25+DSUM(Table224567891011[#All],"Value",$AA$10:$AA$11)</f>
+        <f>R25+DSUM(Table224567891011[#All],"Value",$AB$10:$AB$11)</f>
         <v>0</v>
       </c>
       <c r="S26" s="117">
@@ -3441,8 +3455,9 @@
       <c r="Z26" s="117">
         <v>0.54949999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="15:26">
+      <c r="AA26" s="117"/>
+    </row>
+    <row r="27" spans="15:27">
       <c r="O27" s="137" t="s">
         <v>59</v>
       </c>
@@ -3455,7 +3470,7 @@
         <v>0.6875</v>
       </c>
       <c r="R27" s="3">
-        <f>R26+DSUM(Table22456789101112[#All],"Value",$AA$10:$AA$11)</f>
+        <f>R26+DSUM(Table22456789101112[#All],"Value",$AB$10:$AB$11)</f>
         <v>0</v>
       </c>
       <c r="S27" s="117">
@@ -3485,8 +3500,9 @@
       <c r="Z27" s="117">
         <v>0.59950000000000003</v>
       </c>
-    </row>
-    <row r="28" spans="15:26">
+      <c r="AA27" s="117"/>
+    </row>
+    <row r="28" spans="15:27">
       <c r="O28" s="137" t="s">
         <v>60</v>
       </c>
@@ -3498,7 +3514,7 @@
         <v>0.75</v>
       </c>
       <c r="R28" s="3">
-        <f>R27+DSUM(Table2245678910111213[#All],"Value",$AA$10:$AA$11)</f>
+        <f>R27+DSUM(Table2245678910111213[#All],"Value",$AB$10:$AB$11)</f>
         <v>0</v>
       </c>
       <c r="S28" s="117">
@@ -3528,6 +3544,7 @@
       <c r="Z28" s="117">
         <v>0.76449999999999996</v>
       </c>
+      <c r="AA28" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3544,7 +3561,7 @@
   <dimension ref="A2:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3833,7 +3850,7 @@
   <dimension ref="A2:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4120,7 +4137,7 @@
   <dimension ref="A2:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4413,7 +4430,7 @@
   <dimension ref="A2:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4704,7 +4721,7 @@
   <dimension ref="A2:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5001,7 +5018,7 @@
   <dimension ref="A2:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5291,7 +5308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -7113,7 +7130,7 @@
   <dimension ref="A2:N17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7358,7 +7375,7 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="1"/>
+      <c r="A16" s="5"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:5">
@@ -7407,7 +7424,7 @@
   <dimension ref="A2:O17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7652,7 +7669,7 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="1"/>
+      <c r="A16" s="5"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:5">
@@ -7701,7 +7718,7 @@
   <dimension ref="A2:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7948,7 +7965,7 @@
       </c>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="1"/>
+      <c r="A16" s="5"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:5">
@@ -7997,7 +8014,7 @@
   <dimension ref="A2:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8246,7 +8263,7 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="1"/>
+      <c r="A16" s="5"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:5">
@@ -8295,7 +8312,7 @@
   <dimension ref="A2:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8542,7 +8559,7 @@
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="1"/>
+      <c r="A16" s="5"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:5">
@@ -8591,7 +8608,7 @@
   <dimension ref="A2:N35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8829,7 +8846,7 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="1"/>
+      <c r="A16" s="5"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:5">

</xml_diff>